<commit_message>
add hole depth data, R2 B3 bottle weights
</commit_message>
<xml_diff>
--- a/Data/LeachateData.xlsx
+++ b/Data/LeachateData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredflater/Desktop/Flater_soilColumnAnalysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C70FA36-7606-6A4A-A75A-94F36AD21DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7548E42B-746D-2E46-A8DD-916D8EDA1478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
   </bookViews>
@@ -2817,8 +2817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1978E5-E4E9-6B46-8E5C-BBF3C2484C99}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3972,9 +3972,12 @@
       <c r="D38">
         <v>1000</v>
       </c>
+      <c r="E38">
+        <v>88</v>
+      </c>
       <c r="G38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-88</v>
       </c>
       <c r="I38" t="s">
         <v>231</v>
@@ -3993,9 +3996,12 @@
       <c r="D39">
         <v>1000</v>
       </c>
+      <c r="E39">
+        <v>89</v>
+      </c>
       <c r="G39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-89</v>
       </c>
       <c r="I39" t="s">
         <v>231</v>
@@ -4014,9 +4020,12 @@
       <c r="D40">
         <v>1000</v>
       </c>
+      <c r="E40">
+        <v>88</v>
+      </c>
       <c r="G40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-88</v>
       </c>
       <c r="I40" t="s">
         <v>231</v>
@@ -4035,9 +4044,12 @@
       <c r="D41">
         <v>1000</v>
       </c>
+      <c r="E41">
+        <v>89</v>
+      </c>
       <c r="G41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-89</v>
       </c>
       <c r="I41" t="s">
         <v>231</v>
@@ -4056,9 +4068,12 @@
       <c r="D42">
         <v>1000</v>
       </c>
+      <c r="E42">
+        <v>104</v>
+      </c>
       <c r="G42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-104</v>
       </c>
       <c r="I42" t="s">
         <v>231</v>
@@ -4077,9 +4092,12 @@
       <c r="D43">
         <v>1000</v>
       </c>
+      <c r="E43">
+        <v>89</v>
+      </c>
       <c r="G43">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-89</v>
       </c>
       <c r="I43" t="s">
         <v>231</v>
@@ -4098,9 +4116,12 @@
       <c r="D44">
         <v>1000</v>
       </c>
+      <c r="E44">
+        <v>90</v>
+      </c>
       <c r="G44">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="I44" t="s">
         <v>231</v>
@@ -4119,9 +4140,12 @@
       <c r="D45">
         <v>1000</v>
       </c>
+      <c r="E45">
+        <v>90</v>
+      </c>
       <c r="G45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="I45" t="s">
         <v>231</v>
@@ -4140,9 +4164,12 @@
       <c r="D46">
         <v>1000</v>
       </c>
+      <c r="E46">
+        <v>90</v>
+      </c>
       <c r="G46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="I46" t="s">
         <v>231</v>
@@ -4161,9 +4188,12 @@
       <c r="D47">
         <v>1000</v>
       </c>
+      <c r="E47">
+        <v>88</v>
+      </c>
       <c r="G47">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-88</v>
       </c>
       <c r="I47" t="s">
         <v>231</v>
@@ -4182,9 +4212,12 @@
       <c r="D48">
         <v>1000</v>
       </c>
+      <c r="E48">
+        <v>101</v>
+      </c>
       <c r="G48">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-101</v>
       </c>
       <c r="I48" t="s">
         <v>231</v>
@@ -4203,9 +4236,12 @@
       <c r="D49">
         <v>1000</v>
       </c>
+      <c r="E49">
+        <v>90</v>
+      </c>
       <c r="G49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="I49" t="s">
         <v>231</v>
@@ -4224,9 +4260,12 @@
       <c r="D50">
         <v>1000</v>
       </c>
+      <c r="E50">
+        <v>89</v>
+      </c>
       <c r="G50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-89</v>
       </c>
       <c r="I50" t="s">
         <v>231</v>
@@ -4245,9 +4284,12 @@
       <c r="D51">
         <v>1000</v>
       </c>
+      <c r="E51">
+        <v>89</v>
+      </c>
       <c r="G51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-89</v>
       </c>
       <c r="I51" t="s">
         <v>231</v>
@@ -4266,9 +4308,12 @@
       <c r="D52">
         <v>1000</v>
       </c>
+      <c r="E52">
+        <v>89</v>
+      </c>
       <c r="G52">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-89</v>
       </c>
       <c r="I52" t="s">
         <v>231</v>
@@ -4287,9 +4332,12 @@
       <c r="D53">
         <v>1000</v>
       </c>
+      <c r="E53">
+        <v>88</v>
+      </c>
       <c r="G53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-88</v>
       </c>
       <c r="I53" t="s">
         <v>231</v>
@@ -4308,9 +4356,12 @@
       <c r="D54">
         <v>1000</v>
       </c>
+      <c r="E54">
+        <v>88</v>
+      </c>
       <c r="G54">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-88</v>
       </c>
       <c r="I54" t="s">
         <v>231</v>
@@ -4329,9 +4380,12 @@
       <c r="D55">
         <v>1000</v>
       </c>
+      <c r="E55">
+        <v>89</v>
+      </c>
       <c r="G55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-89</v>
       </c>
       <c r="I55" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
add B3 R3 leachate mass
</commit_message>
<xml_diff>
--- a/Data/LeachateData.xlsx
+++ b/Data/LeachateData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredflater/Desktop/Flater_soilColumnAnalysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7548E42B-746D-2E46-A8DD-916D8EDA1478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135F066D-2027-8F49-9D1D-44432DB3C2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
   </bookViews>
@@ -2817,8 +2817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1978E5-E4E9-6B46-8E5C-BBF3C2484C99}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3975,9 +3975,15 @@
       <c r="E38">
         <v>88</v>
       </c>
+      <c r="F38">
+        <v>772</v>
+      </c>
       <c r="G38">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>684</v>
+      </c>
+      <c r="H38">
+        <v>20210611</v>
       </c>
       <c r="I38" t="s">
         <v>231</v>
@@ -3999,9 +4005,15 @@
       <c r="E39">
         <v>89</v>
       </c>
+      <c r="F39">
+        <v>814</v>
+      </c>
       <c r="G39">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>725</v>
+      </c>
+      <c r="H39">
+        <v>20210611</v>
       </c>
       <c r="I39" t="s">
         <v>231</v>
@@ -4023,9 +4035,15 @@
       <c r="E40">
         <v>88</v>
       </c>
+      <c r="F40">
+        <v>905</v>
+      </c>
       <c r="G40">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>817</v>
+      </c>
+      <c r="H40">
+        <v>20210611</v>
       </c>
       <c r="I40" t="s">
         <v>231</v>
@@ -4047,9 +4065,15 @@
       <c r="E41">
         <v>89</v>
       </c>
+      <c r="F41">
+        <v>843</v>
+      </c>
       <c r="G41">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>754</v>
+      </c>
+      <c r="H41">
+        <v>20210611</v>
       </c>
       <c r="I41" t="s">
         <v>231</v>
@@ -4071,9 +4095,15 @@
       <c r="E42">
         <v>104</v>
       </c>
+      <c r="F42">
+        <v>827</v>
+      </c>
       <c r="G42">
         <f t="shared" si="0"/>
-        <v>-104</v>
+        <v>723</v>
+      </c>
+      <c r="H42">
+        <v>20210611</v>
       </c>
       <c r="I42" t="s">
         <v>231</v>
@@ -4095,9 +4125,15 @@
       <c r="E43">
         <v>89</v>
       </c>
+      <c r="F43">
+        <v>810</v>
+      </c>
       <c r="G43">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>721</v>
+      </c>
+      <c r="H43">
+        <v>20210611</v>
       </c>
       <c r="I43" t="s">
         <v>231</v>
@@ -4119,9 +4155,15 @@
       <c r="E44">
         <v>90</v>
       </c>
+      <c r="F44">
+        <v>847</v>
+      </c>
       <c r="G44">
         <f t="shared" si="0"/>
-        <v>-90</v>
+        <v>757</v>
+      </c>
+      <c r="H44">
+        <v>20210611</v>
       </c>
       <c r="I44" t="s">
         <v>231</v>
@@ -4143,9 +4185,15 @@
       <c r="E45">
         <v>90</v>
       </c>
+      <c r="F45">
+        <v>790</v>
+      </c>
       <c r="G45">
         <f t="shared" si="0"/>
-        <v>-90</v>
+        <v>700</v>
+      </c>
+      <c r="H45">
+        <v>20210611</v>
       </c>
       <c r="I45" t="s">
         <v>231</v>
@@ -4167,9 +4215,15 @@
       <c r="E46">
         <v>90</v>
       </c>
+      <c r="F46">
+        <v>857</v>
+      </c>
       <c r="G46">
         <f t="shared" si="0"/>
-        <v>-90</v>
+        <v>767</v>
+      </c>
+      <c r="H46">
+        <v>20210611</v>
       </c>
       <c r="I46" t="s">
         <v>231</v>
@@ -4191,9 +4245,15 @@
       <c r="E47">
         <v>88</v>
       </c>
+      <c r="F47">
+        <v>833</v>
+      </c>
       <c r="G47">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>745</v>
+      </c>
+      <c r="H47">
+        <v>20210611</v>
       </c>
       <c r="I47" t="s">
         <v>231</v>
@@ -4215,9 +4275,15 @@
       <c r="E48">
         <v>101</v>
       </c>
+      <c r="F48">
+        <v>825</v>
+      </c>
       <c r="G48">
         <f t="shared" si="0"/>
-        <v>-101</v>
+        <v>724</v>
+      </c>
+      <c r="H48">
+        <v>20210611</v>
       </c>
       <c r="I48" t="s">
         <v>231</v>
@@ -4239,9 +4305,15 @@
       <c r="E49">
         <v>90</v>
       </c>
+      <c r="F49">
+        <v>869</v>
+      </c>
       <c r="G49">
         <f t="shared" si="0"/>
-        <v>-90</v>
+        <v>779</v>
+      </c>
+      <c r="H49">
+        <v>20210611</v>
       </c>
       <c r="I49" t="s">
         <v>231</v>
@@ -4263,9 +4335,15 @@
       <c r="E50">
         <v>89</v>
       </c>
+      <c r="F50">
+        <v>868</v>
+      </c>
       <c r="G50">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>779</v>
+      </c>
+      <c r="H50">
+        <v>20210611</v>
       </c>
       <c r="I50" t="s">
         <v>231</v>
@@ -4287,9 +4365,15 @@
       <c r="E51">
         <v>89</v>
       </c>
+      <c r="F51">
+        <v>845</v>
+      </c>
       <c r="G51">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>756</v>
+      </c>
+      <c r="H51">
+        <v>20210611</v>
       </c>
       <c r="I51" t="s">
         <v>231</v>
@@ -4311,9 +4395,15 @@
       <c r="E52">
         <v>89</v>
       </c>
+      <c r="F52">
+        <v>855</v>
+      </c>
       <c r="G52">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>766</v>
+      </c>
+      <c r="H52">
+        <v>20210611</v>
       </c>
       <c r="I52" t="s">
         <v>231</v>
@@ -4335,9 +4425,15 @@
       <c r="E53">
         <v>88</v>
       </c>
+      <c r="F53">
+        <v>854</v>
+      </c>
       <c r="G53">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>766</v>
+      </c>
+      <c r="H53">
+        <v>20210611</v>
       </c>
       <c r="I53" t="s">
         <v>231</v>
@@ -4359,9 +4455,15 @@
       <c r="E54">
         <v>88</v>
       </c>
+      <c r="F54">
+        <v>870</v>
+      </c>
       <c r="G54">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>782</v>
+      </c>
+      <c r="H54">
+        <v>20210611</v>
       </c>
       <c r="I54" t="s">
         <v>231</v>
@@ -4383,9 +4485,15 @@
       <c r="E55">
         <v>89</v>
       </c>
+      <c r="F55">
+        <v>861</v>
+      </c>
       <c r="G55">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>772</v>
+      </c>
+      <c r="H55">
+        <v>20210611</v>
       </c>
       <c r="I55" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
Bottle weights for B1 R3
</commit_message>
<xml_diff>
--- a/Data/LeachateData.xlsx
+++ b/Data/LeachateData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredflater/Desktop/Flater_soilColumnAnalysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135F066D-2027-8F49-9D1D-44432DB3C2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC8DE1D-3FFB-3445-B102-7884D9F99874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Rainfall 1" sheetId="1" r:id="rId1"/>
     <sheet name="Rainfall 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -70,8 +71,26 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={944BE181-8429-0C41-98F4-DAD1FFAEEFEF}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{944BE181-8429-0C41-98F4-DAD1FFAEEFEF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Please make unique name, not start with number, add project name</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="340">
   <si>
     <t>unique sample_id</t>
   </si>
@@ -767,13 +786,337 @@
   </si>
   <si>
     <t>Freezer_F_Shelf_5</t>
+  </si>
+  <si>
+    <t>SSCAMR00163</t>
+  </si>
+  <si>
+    <t>SSCAMR00164</t>
+  </si>
+  <si>
+    <t>SSCAMR00165</t>
+  </si>
+  <si>
+    <t>SSCAMR00166</t>
+  </si>
+  <si>
+    <t>SSCAMR00167</t>
+  </si>
+  <si>
+    <t>SSCAMR00168</t>
+  </si>
+  <si>
+    <t>SSCAMR00169</t>
+  </si>
+  <si>
+    <t>SSCAMR00170</t>
+  </si>
+  <si>
+    <t>SSCAMR00171</t>
+  </si>
+  <si>
+    <t>SSCAMR00172</t>
+  </si>
+  <si>
+    <t>SSCAMR00173</t>
+  </si>
+  <si>
+    <t>SSCAMR00174</t>
+  </si>
+  <si>
+    <t>SSCAMR00175</t>
+  </si>
+  <si>
+    <t>SSCAMR00176</t>
+  </si>
+  <si>
+    <t>SSCAMR00177</t>
+  </si>
+  <si>
+    <t>SSCAMR00178</t>
+  </si>
+  <si>
+    <t>SSCAMR00179</t>
+  </si>
+  <si>
+    <t>SSCAMR00180</t>
+  </si>
+  <si>
+    <t>SSCAMR00181</t>
+  </si>
+  <si>
+    <t>SSCAMR00182</t>
+  </si>
+  <si>
+    <t>SSCAMR00183</t>
+  </si>
+  <si>
+    <t>SSCAMR00184</t>
+  </si>
+  <si>
+    <t>SSCAMR00185</t>
+  </si>
+  <si>
+    <t>SSCAMR00186</t>
+  </si>
+  <si>
+    <t>SSCAMR00187</t>
+  </si>
+  <si>
+    <t>SSCAMR00188</t>
+  </si>
+  <si>
+    <t>SSCAMR00189</t>
+  </si>
+  <si>
+    <t>SSCAMR00190</t>
+  </si>
+  <si>
+    <t>SSCAMR00191</t>
+  </si>
+  <si>
+    <t>SSCAMR00192</t>
+  </si>
+  <si>
+    <t>SSCAMR00193</t>
+  </si>
+  <si>
+    <t>SSCAMR00194</t>
+  </si>
+  <si>
+    <t>SSCAMR00195</t>
+  </si>
+  <si>
+    <t>SSCAMR00196</t>
+  </si>
+  <si>
+    <t>SSCAMR00197</t>
+  </si>
+  <si>
+    <t>SSCAMR00198</t>
+  </si>
+  <si>
+    <t>SSCAMR00199</t>
+  </si>
+  <si>
+    <t>SSCAMR00200</t>
+  </si>
+  <si>
+    <t>SSCAMR00201</t>
+  </si>
+  <si>
+    <t>SSCAMR00202</t>
+  </si>
+  <si>
+    <t>SSCAMR00203</t>
+  </si>
+  <si>
+    <t>SSCAMR00204</t>
+  </si>
+  <si>
+    <t>SSCAMR00205</t>
+  </si>
+  <si>
+    <t>SSCAMR00206</t>
+  </si>
+  <si>
+    <t>SSCAMR00207</t>
+  </si>
+  <si>
+    <t>SSCAMR00208</t>
+  </si>
+  <si>
+    <t>SSCAMR00209</t>
+  </si>
+  <si>
+    <t>SSCAMR00210</t>
+  </si>
+  <si>
+    <t>SSCAMR00211</t>
+  </si>
+  <si>
+    <t>SSCAMR00212</t>
+  </si>
+  <si>
+    <t>SSCAMR00213</t>
+  </si>
+  <si>
+    <t>SSCAMR00214</t>
+  </si>
+  <si>
+    <t>SSCAMR00215</t>
+  </si>
+  <si>
+    <t>SSCAMR00216</t>
+  </si>
+  <si>
+    <t>C01R3</t>
+  </si>
+  <si>
+    <t>C02R3</t>
+  </si>
+  <si>
+    <t>C03R3</t>
+  </si>
+  <si>
+    <t>C04R3</t>
+  </si>
+  <si>
+    <t>C05R3</t>
+  </si>
+  <si>
+    <t>C06R3</t>
+  </si>
+  <si>
+    <t>C07R3</t>
+  </si>
+  <si>
+    <t>C08R3</t>
+  </si>
+  <si>
+    <t>C09R3</t>
+  </si>
+  <si>
+    <t>C10R3</t>
+  </si>
+  <si>
+    <t>C11R3</t>
+  </si>
+  <si>
+    <t>C12R3</t>
+  </si>
+  <si>
+    <t>C13R3</t>
+  </si>
+  <si>
+    <t>C14R3</t>
+  </si>
+  <si>
+    <t>C15R3</t>
+  </si>
+  <si>
+    <t>C16R3</t>
+  </si>
+  <si>
+    <t>C17R3</t>
+  </si>
+  <si>
+    <t>C18R3</t>
+  </si>
+  <si>
+    <t>C19R3</t>
+  </si>
+  <si>
+    <t>C20R3</t>
+  </si>
+  <si>
+    <t>C21R3</t>
+  </si>
+  <si>
+    <t>C22R3</t>
+  </si>
+  <si>
+    <t>C23R3</t>
+  </si>
+  <si>
+    <t>C24R3</t>
+  </si>
+  <si>
+    <t>C25R3</t>
+  </si>
+  <si>
+    <t>C26R3</t>
+  </si>
+  <si>
+    <t>C27R3</t>
+  </si>
+  <si>
+    <t>C28R3</t>
+  </si>
+  <si>
+    <t>C29R3</t>
+  </si>
+  <si>
+    <t>C30R3</t>
+  </si>
+  <si>
+    <t>C31R3</t>
+  </si>
+  <si>
+    <t>C32R3</t>
+  </si>
+  <si>
+    <t>C33R3</t>
+  </si>
+  <si>
+    <t>C34R3</t>
+  </si>
+  <si>
+    <t>C35R3</t>
+  </si>
+  <si>
+    <t>C36R3</t>
+  </si>
+  <si>
+    <t>C37R3</t>
+  </si>
+  <si>
+    <t>C38R3</t>
+  </si>
+  <si>
+    <t>C39R3</t>
+  </si>
+  <si>
+    <t>C40R3</t>
+  </si>
+  <si>
+    <t>C41R3</t>
+  </si>
+  <si>
+    <t>C42R3</t>
+  </si>
+  <si>
+    <t>C43R3</t>
+  </si>
+  <si>
+    <t>C44R3</t>
+  </si>
+  <si>
+    <t>C45R3</t>
+  </si>
+  <si>
+    <t>C46R3</t>
+  </si>
+  <si>
+    <t>C47R3</t>
+  </si>
+  <si>
+    <t>C48R3</t>
+  </si>
+  <si>
+    <t>C49R3</t>
+  </si>
+  <si>
+    <t>C50R3</t>
+  </si>
+  <si>
+    <t>C51R3</t>
+  </si>
+  <si>
+    <t>C52R3</t>
+  </si>
+  <si>
+    <t>C53R3</t>
+  </si>
+  <si>
+    <t>C54R3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -793,6 +1136,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -836,13 +1185,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1177,6 +1527,14 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2019-08-30T18:32:40.31" personId="{8719274A-2B76-AD41-A8F1-7203866E8D23}" id="{944BE181-8429-0C41-98F4-DAD1FFAEEFEF}">
+    <text>Please make unique name, not start with number, add project name</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A39224-C7A3-DC45-833D-204FCB526563}">
   <dimension ref="A1:M55"/>
@@ -2817,8 +3175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1978E5-E4E9-6B46-8E5C-BBF3C2484C99}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4504,4 +4862,887 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7CF24D-EF41-5241-906E-DAD6D3AC4CE4}">
+  <dimension ref="A1:M55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <v>88</v>
+      </c>
+      <c r="I2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>90</v>
+      </c>
+      <c r="I3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>89</v>
+      </c>
+      <c r="I4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E5">
+        <v>89</v>
+      </c>
+      <c r="I5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E6">
+        <v>89</v>
+      </c>
+      <c r="I6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E7">
+        <v>105</v>
+      </c>
+      <c r="I7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B8" t="s">
+        <v>292</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E8">
+        <v>90</v>
+      </c>
+      <c r="I8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B9" t="s">
+        <v>293</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E9">
+        <v>89</v>
+      </c>
+      <c r="I9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B10" t="s">
+        <v>294</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E10">
+        <v>88</v>
+      </c>
+      <c r="I10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B11" t="s">
+        <v>295</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E11">
+        <v>88</v>
+      </c>
+      <c r="I11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" t="s">
+        <v>296</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E12">
+        <v>87</v>
+      </c>
+      <c r="I12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B13" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E13">
+        <v>87</v>
+      </c>
+      <c r="I13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B14" t="s">
+        <v>298</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E14">
+        <v>88</v>
+      </c>
+      <c r="I14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B15" t="s">
+        <v>299</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E15">
+        <v>88</v>
+      </c>
+      <c r="I15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" t="s">
+        <v>300</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E16">
+        <v>89</v>
+      </c>
+      <c r="I16" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B17" t="s">
+        <v>301</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E17">
+        <v>88</v>
+      </c>
+      <c r="I17" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B18" t="s">
+        <v>302</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E18">
+        <v>88</v>
+      </c>
+      <c r="I18" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B19" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E19">
+        <v>87</v>
+      </c>
+      <c r="I19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B20" t="s">
+        <v>304</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I20" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B21" t="s">
+        <v>305</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I21" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B22" t="s">
+        <v>306</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23" t="s">
+        <v>307</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I23" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B24" t="s">
+        <v>308</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I24" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B25" t="s">
+        <v>309</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I25" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B26" t="s">
+        <v>310</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I26" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B27" t="s">
+        <v>311</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I27" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B28" t="s">
+        <v>312</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I28" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B29" t="s">
+        <v>313</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I29" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B30" t="s">
+        <v>314</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I30" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B31" t="s">
+        <v>315</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I31" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B32" t="s">
+        <v>316</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I32" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B33" t="s">
+        <v>317</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I33" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B34" t="s">
+        <v>318</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I34" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B35" t="s">
+        <v>319</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I35" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B36" t="s">
+        <v>320</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I36" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B37" t="s">
+        <v>321</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I37" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B38" t="s">
+        <v>322</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I38" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B39" t="s">
+        <v>323</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I39" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B40" t="s">
+        <v>324</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I40" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B41" t="s">
+        <v>325</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I41" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B42" t="s">
+        <v>326</v>
+      </c>
+      <c r="D42" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I42" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B43" t="s">
+        <v>327</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I43" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B44" t="s">
+        <v>328</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I44" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B45" t="s">
+        <v>329</v>
+      </c>
+      <c r="D45" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I45" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B46" t="s">
+        <v>330</v>
+      </c>
+      <c r="D46" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I46" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B47" t="s">
+        <v>331</v>
+      </c>
+      <c r="D47" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I47" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B48" t="s">
+        <v>332</v>
+      </c>
+      <c r="D48" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I48" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B49" t="s">
+        <v>333</v>
+      </c>
+      <c r="D49" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I49" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B50" t="s">
+        <v>334</v>
+      </c>
+      <c r="D50" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I50" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B51" t="s">
+        <v>335</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I51" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B52" t="s">
+        <v>336</v>
+      </c>
+      <c r="D52" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I52" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B53" t="s">
+        <v>337</v>
+      </c>
+      <c r="D53" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I53" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B54" t="s">
+        <v>338</v>
+      </c>
+      <c r="D54" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I54" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B55" t="s">
+        <v>339</v>
+      </c>
+      <c r="D55" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I55" t="s">
+        <v>231</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
B2 R3 leachate weights and associated data
</commit_message>
<xml_diff>
--- a/Data/LeachateData.xlsx
+++ b/Data/LeachateData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredflater/Desktop/Flater_soilColumnAnalysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC8DE1D-3FFB-3445-B102-7884D9F99874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEF1AE8-91C4-414B-99E1-060D37EDDC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Rainfall 1" sheetId="1" r:id="rId1"/>
     <sheet name="Rainfall 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Rainfall 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -1116,7 +1116,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1136,12 +1136,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -4869,7 +4863,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4937,11 +4931,24 @@
       <c r="B2" t="s">
         <v>286</v>
       </c>
+      <c r="C2">
+        <v>20210614</v>
+      </c>
       <c r="D2" s="4">
         <v>1000</v>
       </c>
       <c r="E2">
         <v>88</v>
+      </c>
+      <c r="F2">
+        <v>906</v>
+      </c>
+      <c r="G2">
+        <f>F2-E2</f>
+        <v>818</v>
+      </c>
+      <c r="H2">
+        <v>20210614</v>
       </c>
       <c r="I2" t="s">
         <v>231</v>
@@ -4954,11 +4961,24 @@
       <c r="B3" t="s">
         <v>287</v>
       </c>
+      <c r="C3">
+        <v>20210614</v>
+      </c>
       <c r="D3" s="4">
         <v>1000</v>
       </c>
       <c r="E3">
         <v>90</v>
+      </c>
+      <c r="F3">
+        <v>782</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G19" si="0">F3-E3</f>
+        <v>692</v>
+      </c>
+      <c r="H3">
+        <v>20210614</v>
       </c>
       <c r="I3" t="s">
         <v>231</v>
@@ -4971,11 +4991,24 @@
       <c r="B4" t="s">
         <v>288</v>
       </c>
+      <c r="C4">
+        <v>20210614</v>
+      </c>
       <c r="D4" s="4">
         <v>1000</v>
       </c>
       <c r="E4">
         <v>89</v>
+      </c>
+      <c r="F4">
+        <v>810</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>721</v>
+      </c>
+      <c r="H4">
+        <v>20210614</v>
       </c>
       <c r="I4" t="s">
         <v>231</v>
@@ -4988,11 +5021,24 @@
       <c r="B5" t="s">
         <v>289</v>
       </c>
+      <c r="C5">
+        <v>20210614</v>
+      </c>
       <c r="D5" s="4">
         <v>1000</v>
       </c>
       <c r="E5">
         <v>89</v>
+      </c>
+      <c r="F5">
+        <v>880</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>791</v>
+      </c>
+      <c r="H5">
+        <v>20210614</v>
       </c>
       <c r="I5" t="s">
         <v>231</v>
@@ -5005,11 +5051,24 @@
       <c r="B6" t="s">
         <v>290</v>
       </c>
+      <c r="C6">
+        <v>20210614</v>
+      </c>
       <c r="D6" s="4">
         <v>1000</v>
       </c>
       <c r="E6">
         <v>89</v>
+      </c>
+      <c r="F6">
+        <v>794</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>705</v>
+      </c>
+      <c r="H6">
+        <v>20210614</v>
       </c>
       <c r="I6" t="s">
         <v>231</v>
@@ -5022,11 +5081,24 @@
       <c r="B7" t="s">
         <v>291</v>
       </c>
+      <c r="C7">
+        <v>20210614</v>
+      </c>
       <c r="D7" s="4">
         <v>1000</v>
       </c>
       <c r="E7">
         <v>105</v>
+      </c>
+      <c r="F7">
+        <v>833</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>728</v>
+      </c>
+      <c r="H7">
+        <v>20210614</v>
       </c>
       <c r="I7" t="s">
         <v>231</v>
@@ -5039,11 +5111,24 @@
       <c r="B8" t="s">
         <v>292</v>
       </c>
+      <c r="C8">
+        <v>20210614</v>
+      </c>
       <c r="D8" s="4">
         <v>1000</v>
       </c>
       <c r="E8">
         <v>90</v>
+      </c>
+      <c r="F8">
+        <v>882</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>792</v>
+      </c>
+      <c r="H8">
+        <v>20210614</v>
       </c>
       <c r="I8" t="s">
         <v>231</v>
@@ -5056,11 +5141,24 @@
       <c r="B9" t="s">
         <v>293</v>
       </c>
+      <c r="C9">
+        <v>20210614</v>
+      </c>
       <c r="D9" s="4">
         <v>1000</v>
       </c>
       <c r="E9">
         <v>89</v>
+      </c>
+      <c r="F9">
+        <v>788</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>699</v>
+      </c>
+      <c r="H9">
+        <v>20210614</v>
       </c>
       <c r="I9" t="s">
         <v>231</v>
@@ -5073,11 +5171,24 @@
       <c r="B10" t="s">
         <v>294</v>
       </c>
+      <c r="C10">
+        <v>20210614</v>
+      </c>
       <c r="D10" s="4">
         <v>1000</v>
       </c>
       <c r="E10">
         <v>88</v>
+      </c>
+      <c r="F10">
+        <v>829</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>741</v>
+      </c>
+      <c r="H10">
+        <v>20210614</v>
       </c>
       <c r="I10" t="s">
         <v>231</v>
@@ -5090,11 +5201,24 @@
       <c r="B11" t="s">
         <v>295</v>
       </c>
+      <c r="C11">
+        <v>20210614</v>
+      </c>
       <c r="D11" s="4">
         <v>1000</v>
       </c>
       <c r="E11">
         <v>88</v>
+      </c>
+      <c r="F11">
+        <v>850</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>762</v>
+      </c>
+      <c r="H11">
+        <v>20210614</v>
       </c>
       <c r="I11" t="s">
         <v>231</v>
@@ -5107,11 +5231,24 @@
       <c r="B12" t="s">
         <v>296</v>
       </c>
+      <c r="C12">
+        <v>20210614</v>
+      </c>
       <c r="D12" s="4">
         <v>1000</v>
       </c>
       <c r="E12">
         <v>87</v>
+      </c>
+      <c r="F12">
+        <v>915</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>828</v>
+      </c>
+      <c r="H12">
+        <v>20210614</v>
       </c>
       <c r="I12" t="s">
         <v>231</v>
@@ -5124,11 +5261,24 @@
       <c r="B13" t="s">
         <v>297</v>
       </c>
+      <c r="C13">
+        <v>20210614</v>
+      </c>
       <c r="D13" s="4">
         <v>1000</v>
       </c>
       <c r="E13">
         <v>87</v>
+      </c>
+      <c r="F13">
+        <v>854</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>767</v>
+      </c>
+      <c r="H13">
+        <v>20210614</v>
       </c>
       <c r="I13" t="s">
         <v>231</v>
@@ -5141,11 +5291,24 @@
       <c r="B14" t="s">
         <v>298</v>
       </c>
+      <c r="C14">
+        <v>20210614</v>
+      </c>
       <c r="D14" s="4">
         <v>1000</v>
       </c>
       <c r="E14">
         <v>88</v>
+      </c>
+      <c r="F14">
+        <v>840</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>752</v>
+      </c>
+      <c r="H14">
+        <v>20210614</v>
       </c>
       <c r="I14" t="s">
         <v>231</v>
@@ -5158,11 +5321,24 @@
       <c r="B15" t="s">
         <v>299</v>
       </c>
+      <c r="C15">
+        <v>20210614</v>
+      </c>
       <c r="D15" s="4">
         <v>1000</v>
       </c>
       <c r="E15">
         <v>88</v>
+      </c>
+      <c r="F15">
+        <v>852</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>764</v>
+      </c>
+      <c r="H15">
+        <v>20210614</v>
       </c>
       <c r="I15" t="s">
         <v>231</v>
@@ -5175,11 +5351,24 @@
       <c r="B16" t="s">
         <v>300</v>
       </c>
+      <c r="C16">
+        <v>20210614</v>
+      </c>
       <c r="D16" s="4">
         <v>1000</v>
       </c>
       <c r="E16">
         <v>89</v>
+      </c>
+      <c r="F16">
+        <v>887</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>798</v>
+      </c>
+      <c r="H16">
+        <v>20210614</v>
       </c>
       <c r="I16" t="s">
         <v>231</v>
@@ -5192,11 +5381,24 @@
       <c r="B17" t="s">
         <v>301</v>
       </c>
+      <c r="C17">
+        <v>20210614</v>
+      </c>
       <c r="D17" s="4">
         <v>1000</v>
       </c>
       <c r="E17">
         <v>88</v>
+      </c>
+      <c r="F17">
+        <v>884</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>796</v>
+      </c>
+      <c r="H17">
+        <v>20210614</v>
       </c>
       <c r="I17" t="s">
         <v>231</v>
@@ -5209,11 +5411,24 @@
       <c r="B18" t="s">
         <v>302</v>
       </c>
+      <c r="C18">
+        <v>20210614</v>
+      </c>
       <c r="D18" s="4">
         <v>1000</v>
       </c>
       <c r="E18">
         <v>88</v>
+      </c>
+      <c r="F18">
+        <v>895</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>807</v>
+      </c>
+      <c r="H18">
+        <v>20210614</v>
       </c>
       <c r="I18" t="s">
         <v>231</v>
@@ -5226,11 +5441,24 @@
       <c r="B19" t="s">
         <v>303</v>
       </c>
+      <c r="C19">
+        <v>20210614</v>
+      </c>
       <c r="D19" s="4">
         <v>1000</v>
       </c>
       <c r="E19">
         <v>87</v>
+      </c>
+      <c r="F19">
+        <v>771</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>684</v>
+      </c>
+      <c r="H19">
+        <v>20210614</v>
       </c>
       <c r="I19" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
B2 R3 bottle mass
</commit_message>
<xml_diff>
--- a/Data/LeachateData.xlsx
+++ b/Data/LeachateData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredflater/Desktop/Flater_soilColumnAnalysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEF1AE8-91C4-414B-99E1-060D37EDDC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA42C5C-38F8-F041-9549-A84392F6EAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
   </bookViews>
@@ -4863,7 +4863,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5471,8 +5471,14 @@
       <c r="B20" t="s">
         <v>304</v>
       </c>
+      <c r="C20">
+        <v>20210616</v>
+      </c>
       <c r="D20" s="4">
         <v>1000</v>
+      </c>
+      <c r="E20">
+        <v>89</v>
       </c>
       <c r="I20" t="s">
         <v>231</v>
@@ -5485,8 +5491,14 @@
       <c r="B21" t="s">
         <v>305</v>
       </c>
+      <c r="C21">
+        <v>20210616</v>
+      </c>
       <c r="D21" s="4">
         <v>1000</v>
+      </c>
+      <c r="E21">
+        <v>89</v>
       </c>
       <c r="I21" t="s">
         <v>231</v>
@@ -5499,8 +5511,14 @@
       <c r="B22" t="s">
         <v>306</v>
       </c>
+      <c r="C22">
+        <v>20210616</v>
+      </c>
       <c r="D22" s="4">
         <v>1000</v>
+      </c>
+      <c r="E22">
+        <v>88</v>
       </c>
       <c r="I22" t="s">
         <v>231</v>
@@ -5513,8 +5531,14 @@
       <c r="B23" t="s">
         <v>307</v>
       </c>
+      <c r="C23">
+        <v>20210616</v>
+      </c>
       <c r="D23" s="4">
         <v>1000</v>
+      </c>
+      <c r="E23">
+        <v>89</v>
       </c>
       <c r="I23" t="s">
         <v>231</v>
@@ -5527,8 +5551,14 @@
       <c r="B24" t="s">
         <v>308</v>
       </c>
+      <c r="C24">
+        <v>20210616</v>
+      </c>
       <c r="D24" s="4">
         <v>1000</v>
+      </c>
+      <c r="E24">
+        <v>89</v>
       </c>
       <c r="I24" t="s">
         <v>231</v>
@@ -5541,8 +5571,14 @@
       <c r="B25" t="s">
         <v>309</v>
       </c>
+      <c r="C25">
+        <v>20210616</v>
+      </c>
       <c r="D25" s="4">
         <v>1000</v>
+      </c>
+      <c r="E25">
+        <v>88</v>
       </c>
       <c r="I25" t="s">
         <v>231</v>
@@ -5555,8 +5591,14 @@
       <c r="B26" t="s">
         <v>310</v>
       </c>
+      <c r="C26">
+        <v>20210616</v>
+      </c>
       <c r="D26" s="4">
         <v>1000</v>
+      </c>
+      <c r="E26">
+        <v>104</v>
       </c>
       <c r="I26" t="s">
         <v>231</v>
@@ -5569,8 +5611,14 @@
       <c r="B27" t="s">
         <v>311</v>
       </c>
+      <c r="C27">
+        <v>20210616</v>
+      </c>
       <c r="D27" s="4">
         <v>1000</v>
+      </c>
+      <c r="E27">
+        <v>88</v>
       </c>
       <c r="I27" t="s">
         <v>231</v>
@@ -5583,8 +5631,14 @@
       <c r="B28" t="s">
         <v>312</v>
       </c>
+      <c r="C28">
+        <v>20210616</v>
+      </c>
       <c r="D28" s="4">
         <v>1000</v>
+      </c>
+      <c r="E28">
+        <v>89</v>
       </c>
       <c r="I28" t="s">
         <v>231</v>
@@ -5597,8 +5651,14 @@
       <c r="B29" t="s">
         <v>313</v>
       </c>
+      <c r="C29">
+        <v>20210616</v>
+      </c>
       <c r="D29" s="4">
         <v>1000</v>
+      </c>
+      <c r="E29">
+        <v>87</v>
       </c>
       <c r="I29" t="s">
         <v>231</v>
@@ -5611,8 +5671,14 @@
       <c r="B30" t="s">
         <v>314</v>
       </c>
+      <c r="C30">
+        <v>20210616</v>
+      </c>
       <c r="D30" s="4">
         <v>1000</v>
+      </c>
+      <c r="E30">
+        <v>101</v>
       </c>
       <c r="I30" t="s">
         <v>231</v>
@@ -5625,8 +5691,14 @@
       <c r="B31" t="s">
         <v>315</v>
       </c>
+      <c r="C31">
+        <v>20210616</v>
+      </c>
       <c r="D31" s="4">
         <v>1000</v>
+      </c>
+      <c r="E31">
+        <v>90</v>
       </c>
       <c r="I31" t="s">
         <v>231</v>
@@ -5639,8 +5711,14 @@
       <c r="B32" t="s">
         <v>316</v>
       </c>
+      <c r="C32">
+        <v>20210616</v>
+      </c>
       <c r="D32" s="4">
         <v>1000</v>
+      </c>
+      <c r="E32">
+        <v>89</v>
       </c>
       <c r="I32" t="s">
         <v>231</v>
@@ -5653,8 +5731,14 @@
       <c r="B33" t="s">
         <v>317</v>
       </c>
+      <c r="C33">
+        <v>20210616</v>
+      </c>
       <c r="D33" s="4">
         <v>1000</v>
+      </c>
+      <c r="E33">
+        <v>88</v>
       </c>
       <c r="I33" t="s">
         <v>231</v>
@@ -5667,8 +5751,14 @@
       <c r="B34" t="s">
         <v>318</v>
       </c>
+      <c r="C34">
+        <v>20210616</v>
+      </c>
       <c r="D34" s="4">
         <v>1000</v>
+      </c>
+      <c r="E34">
+        <v>89</v>
       </c>
       <c r="I34" t="s">
         <v>231</v>
@@ -5681,8 +5771,14 @@
       <c r="B35" t="s">
         <v>319</v>
       </c>
+      <c r="C35">
+        <v>20210616</v>
+      </c>
       <c r="D35" s="4">
         <v>1000</v>
+      </c>
+      <c r="E35">
+        <v>88</v>
       </c>
       <c r="I35" t="s">
         <v>231</v>
@@ -5695,8 +5791,14 @@
       <c r="B36" t="s">
         <v>320</v>
       </c>
+      <c r="C36">
+        <v>20210616</v>
+      </c>
       <c r="D36" s="4">
         <v>1000</v>
+      </c>
+      <c r="E36">
+        <v>89</v>
       </c>
       <c r="I36" t="s">
         <v>231</v>
@@ -5709,8 +5811,14 @@
       <c r="B37" t="s">
         <v>321</v>
       </c>
+      <c r="C37">
+        <v>20210616</v>
+      </c>
       <c r="D37" s="4">
         <v>1000</v>
+      </c>
+      <c r="E37">
+        <v>89</v>
       </c>
       <c r="I37" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
color slope in leachate data
</commit_message>
<xml_diff>
--- a/Data/LeachateData.xlsx
+++ b/Data/LeachateData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredflater/Desktop/Flater_soilColumnAnalysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA9B137-6106-724A-B99E-A9F796B98C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6679771F-215A-814A-AA54-127BD4F8FBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
   </bookViews>
@@ -1466,7 +1466,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1483,6 +1483,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1526,7 +1532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1537,6 +1543,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7736,7 +7743,7 @@
   <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7857,7 +7864,7 @@
         <v>834</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I19" si="0">H3-G3</f>
+        <f t="shared" ref="I3:I55" si="0">H3-G3</f>
         <v>745</v>
       </c>
       <c r="J3" s="2">
@@ -8521,17 +8528,28 @@
       <c r="C20" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E20" s="2">
         <v>4</v>
       </c>
       <c r="F20" s="7">
         <v>1000</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="G20" s="8">
+        <v>100</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J20" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K20" s="2" t="s">
         <v>230</v>
       </c>
@@ -8550,17 +8568,28 @@
       <c r="C21" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E21" s="2">
         <v>4</v>
       </c>
       <c r="F21" s="7">
         <v>1000</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="G21" s="8">
+        <v>100</v>
+      </c>
+      <c r="H21" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J21" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K21" s="2" t="s">
         <v>230</v>
       </c>
@@ -8579,17 +8608,28 @@
       <c r="C22" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E22" s="2">
         <v>4</v>
       </c>
       <c r="F22" s="7">
         <v>1000</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="G22" s="8">
+        <v>100</v>
+      </c>
+      <c r="H22" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J22" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K22" s="2" t="s">
         <v>230</v>
       </c>
@@ -8608,17 +8648,28 @@
       <c r="C23" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E23" s="2">
         <v>4</v>
       </c>
       <c r="F23" s="7">
         <v>1000</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="G23" s="8">
+        <v>100</v>
+      </c>
+      <c r="H23" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J23" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K23" s="2" t="s">
         <v>230</v>
       </c>
@@ -8637,17 +8688,28 @@
       <c r="C24" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E24" s="2">
         <v>4</v>
       </c>
       <c r="F24" s="7">
         <v>1000</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="G24" s="8">
+        <v>100</v>
+      </c>
+      <c r="H24" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J24" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K24" s="2" t="s">
         <v>230</v>
       </c>
@@ -8666,17 +8728,28 @@
       <c r="C25" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E25" s="2">
         <v>4</v>
       </c>
       <c r="F25" s="7">
         <v>1000</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="G25" s="8">
+        <v>100</v>
+      </c>
+      <c r="H25" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J25" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K25" s="2" t="s">
         <v>230</v>
       </c>
@@ -8695,17 +8768,28 @@
       <c r="C26" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E26" s="2">
         <v>4</v>
       </c>
       <c r="F26" s="7">
         <v>1000</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+      <c r="G26" s="8">
+        <v>100</v>
+      </c>
+      <c r="H26" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J26" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K26" s="2" t="s">
         <v>230</v>
       </c>
@@ -8724,17 +8808,28 @@
       <c r="C27" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E27" s="2">
         <v>4</v>
       </c>
       <c r="F27" s="7">
         <v>1000</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
+      <c r="G27" s="8">
+        <v>100</v>
+      </c>
+      <c r="H27" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J27" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K27" s="2" t="s">
         <v>230</v>
       </c>
@@ -8753,17 +8848,28 @@
       <c r="C28" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E28" s="2">
         <v>4</v>
       </c>
       <c r="F28" s="7">
         <v>1000</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
+      <c r="G28" s="8">
+        <v>100</v>
+      </c>
+      <c r="H28" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J28" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K28" s="2" t="s">
         <v>230</v>
       </c>
@@ -8782,17 +8888,28 @@
       <c r="C29" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E29" s="2">
         <v>4</v>
       </c>
       <c r="F29" s="7">
         <v>1000</v>
       </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+      <c r="G29" s="8">
+        <v>100</v>
+      </c>
+      <c r="H29" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J29" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K29" s="2" t="s">
         <v>230</v>
       </c>
@@ -8811,17 +8928,28 @@
       <c r="C30" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E30" s="2">
         <v>4</v>
       </c>
       <c r="F30" s="7">
         <v>1000</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+      <c r="G30" s="8">
+        <v>100</v>
+      </c>
+      <c r="H30" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J30" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K30" s="2" t="s">
         <v>230</v>
       </c>
@@ -8840,17 +8968,28 @@
       <c r="C31" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E31" s="2">
         <v>4</v>
       </c>
       <c r="F31" s="7">
         <v>1000</v>
       </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
+      <c r="G31" s="8">
+        <v>100</v>
+      </c>
+      <c r="H31" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J31" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K31" s="2" t="s">
         <v>230</v>
       </c>
@@ -8869,17 +9008,28 @@
       <c r="C32" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E32" s="2">
         <v>4</v>
       </c>
       <c r="F32" s="7">
         <v>1000</v>
       </c>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
+      <c r="G32" s="8">
+        <v>100</v>
+      </c>
+      <c r="H32" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J32" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K32" s="2" t="s">
         <v>230</v>
       </c>
@@ -8898,17 +9048,28 @@
       <c r="C33" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E33" s="2">
         <v>4</v>
       </c>
       <c r="F33" s="7">
         <v>1000</v>
       </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
+      <c r="G33" s="8">
+        <v>100</v>
+      </c>
+      <c r="H33" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J33" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K33" s="2" t="s">
         <v>230</v>
       </c>
@@ -8927,17 +9088,28 @@
       <c r="C34" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E34" s="2">
         <v>4</v>
       </c>
       <c r="F34" s="7">
         <v>1000</v>
       </c>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
+      <c r="G34" s="8">
+        <v>100</v>
+      </c>
+      <c r="H34" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J34" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K34" s="2" t="s">
         <v>230</v>
       </c>
@@ -8956,17 +9128,28 @@
       <c r="C35" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E35" s="2">
         <v>4</v>
       </c>
       <c r="F35" s="7">
         <v>1000</v>
       </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
+      <c r="G35" s="8">
+        <v>100</v>
+      </c>
+      <c r="H35" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J35" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K35" s="2" t="s">
         <v>230</v>
       </c>
@@ -8985,17 +9168,28 @@
       <c r="C36" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E36" s="2">
         <v>4</v>
       </c>
       <c r="F36" s="7">
         <v>1000</v>
       </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
+      <c r="G36" s="8">
+        <v>100</v>
+      </c>
+      <c r="H36" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J36" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K36" s="2" t="s">
         <v>230</v>
       </c>
@@ -9014,17 +9208,28 @@
       <c r="C37" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D37" s="2"/>
+      <c r="D37" s="2">
+        <v>20210622</v>
+      </c>
       <c r="E37" s="2">
         <v>4</v>
       </c>
       <c r="F37" s="7">
         <v>1000</v>
       </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
+      <c r="G37" s="8">
+        <v>100</v>
+      </c>
+      <c r="H37" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J37" s="2">
+        <v>20210622</v>
+      </c>
       <c r="K37" s="2" t="s">
         <v>230</v>
       </c>
@@ -9043,17 +9248,28 @@
       <c r="C38" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D38" s="2"/>
+      <c r="D38" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E38" s="2">
         <v>4</v>
       </c>
       <c r="F38" s="7">
         <v>1000</v>
       </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
+      <c r="G38" s="8">
+        <v>100</v>
+      </c>
+      <c r="H38" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J38" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K38" s="2" t="s">
         <v>230</v>
       </c>
@@ -9072,17 +9288,28 @@
       <c r="C39" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="D39" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E39" s="2">
         <v>4</v>
       </c>
       <c r="F39" s="7">
         <v>1000</v>
       </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
+      <c r="G39" s="8">
+        <v>100</v>
+      </c>
+      <c r="H39" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J39" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K39" s="2" t="s">
         <v>230</v>
       </c>
@@ -9101,17 +9328,28 @@
       <c r="C40" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="D40" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E40" s="2">
         <v>4</v>
       </c>
       <c r="F40" s="7">
         <v>1000</v>
       </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
+      <c r="G40" s="8">
+        <v>100</v>
+      </c>
+      <c r="H40" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J40" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K40" s="2" t="s">
         <v>230</v>
       </c>
@@ -9130,17 +9368,28 @@
       <c r="C41" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="D41" s="2"/>
+      <c r="D41" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E41" s="2">
         <v>4</v>
       </c>
       <c r="F41" s="7">
         <v>1000</v>
       </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
+      <c r="G41" s="8">
+        <v>100</v>
+      </c>
+      <c r="H41" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J41" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K41" s="2" t="s">
         <v>230</v>
       </c>
@@ -9159,17 +9408,28 @@
       <c r="C42" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="D42" s="2"/>
+      <c r="D42" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E42" s="2">
         <v>4</v>
       </c>
       <c r="F42" s="7">
         <v>1000</v>
       </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
+      <c r="G42" s="8">
+        <v>100</v>
+      </c>
+      <c r="H42" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J42" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K42" s="2" t="s">
         <v>230</v>
       </c>
@@ -9188,17 +9448,28 @@
       <c r="C43" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="D43" s="2"/>
+      <c r="D43" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E43" s="2">
         <v>4</v>
       </c>
       <c r="F43" s="7">
         <v>1000</v>
       </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
+      <c r="G43" s="8">
+        <v>100</v>
+      </c>
+      <c r="H43" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J43" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K43" s="2" t="s">
         <v>230</v>
       </c>
@@ -9217,17 +9488,28 @@
       <c r="C44" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D44" s="2"/>
+      <c r="D44" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E44" s="2">
         <v>4</v>
       </c>
       <c r="F44" s="7">
         <v>1000</v>
       </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
+      <c r="G44" s="8">
+        <v>100</v>
+      </c>
+      <c r="H44" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J44" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K44" s="2" t="s">
         <v>230</v>
       </c>
@@ -9246,17 +9528,28 @@
       <c r="C45" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D45" s="2"/>
+      <c r="D45" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E45" s="2">
         <v>4</v>
       </c>
       <c r="F45" s="7">
         <v>1000</v>
       </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
+      <c r="G45" s="8">
+        <v>100</v>
+      </c>
+      <c r="H45" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J45" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K45" s="2" t="s">
         <v>230</v>
       </c>
@@ -9275,17 +9568,28 @@
       <c r="C46" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="D46" s="2"/>
+      <c r="D46" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E46" s="2">
         <v>4</v>
       </c>
       <c r="F46" s="7">
         <v>1000</v>
       </c>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
+      <c r="G46" s="8">
+        <v>100</v>
+      </c>
+      <c r="H46" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J46" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K46" s="2" t="s">
         <v>230</v>
       </c>
@@ -9304,17 +9608,28 @@
       <c r="C47" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D47" s="2"/>
+      <c r="D47" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E47" s="2">
         <v>4</v>
       </c>
       <c r="F47" s="7">
         <v>1000</v>
       </c>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
+      <c r="G47" s="8">
+        <v>100</v>
+      </c>
+      <c r="H47" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J47" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K47" s="2" t="s">
         <v>230</v>
       </c>
@@ -9333,17 +9648,28 @@
       <c r="C48" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="D48" s="2"/>
+      <c r="D48" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E48" s="2">
         <v>4</v>
       </c>
       <c r="F48" s="7">
         <v>1000</v>
       </c>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
+      <c r="G48" s="8">
+        <v>100</v>
+      </c>
+      <c r="H48" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J48" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K48" s="2" t="s">
         <v>230</v>
       </c>
@@ -9362,17 +9688,28 @@
       <c r="C49" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D49" s="2"/>
+      <c r="D49" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E49" s="2">
         <v>4</v>
       </c>
       <c r="F49" s="7">
         <v>1000</v>
       </c>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
+      <c r="G49" s="8">
+        <v>100</v>
+      </c>
+      <c r="H49" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J49" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K49" s="2" t="s">
         <v>230</v>
       </c>
@@ -9391,17 +9728,28 @@
       <c r="C50" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="D50" s="2"/>
+      <c r="D50" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E50" s="2">
         <v>4</v>
       </c>
       <c r="F50" s="7">
         <v>1000</v>
       </c>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
+      <c r="G50" s="8">
+        <v>100</v>
+      </c>
+      <c r="H50" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J50" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K50" s="2" t="s">
         <v>230</v>
       </c>
@@ -9420,17 +9768,28 @@
       <c r="C51" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="D51" s="2"/>
+      <c r="D51" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E51" s="2">
         <v>4</v>
       </c>
       <c r="F51" s="7">
         <v>1000</v>
       </c>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
+      <c r="G51" s="8">
+        <v>100</v>
+      </c>
+      <c r="H51" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J51" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K51" s="2" t="s">
         <v>230</v>
       </c>
@@ -9449,17 +9808,28 @@
       <c r="C52" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="D52" s="2"/>
+      <c r="D52" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E52" s="2">
         <v>4</v>
       </c>
       <c r="F52" s="7">
         <v>1000</v>
       </c>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
+      <c r="G52" s="8">
+        <v>100</v>
+      </c>
+      <c r="H52" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J52" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K52" s="2" t="s">
         <v>230</v>
       </c>
@@ -9478,17 +9848,28 @@
       <c r="C53" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E53" s="2">
         <v>4</v>
       </c>
       <c r="F53" s="7">
         <v>1000</v>
       </c>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
+      <c r="G53" s="8">
+        <v>100</v>
+      </c>
+      <c r="H53" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J53" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K53" s="2" t="s">
         <v>230</v>
       </c>
@@ -9507,17 +9888,28 @@
       <c r="C54" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="D54" s="2"/>
+      <c r="D54" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E54" s="2">
         <v>4</v>
       </c>
       <c r="F54" s="7">
         <v>1000</v>
       </c>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
+      <c r="G54" s="8">
+        <v>100</v>
+      </c>
+      <c r="H54" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J54" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K54" s="2" t="s">
         <v>230</v>
       </c>
@@ -9536,17 +9928,28 @@
       <c r="C55" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="D55" s="2"/>
+      <c r="D55" s="2">
+        <v>20210624</v>
+      </c>
       <c r="E55" s="2">
         <v>4</v>
       </c>
       <c r="F55" s="7">
         <v>1000</v>
       </c>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
+      <c r="G55" s="8">
+        <v>100</v>
+      </c>
+      <c r="H55" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I55" s="2">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="J55" s="2">
+        <v>20210624</v>
+      </c>
       <c r="K55" s="2" t="s">
         <v>230</v>
       </c>

</xml_diff>

<commit_message>
update plot code, cleaning it up
</commit_message>
<xml_diff>
--- a/Data/LeachateData.xlsx
+++ b/Data/LeachateData.xlsx
@@ -5,34 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredflater/Desktop/Flater_soilColumnAnalysis/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredflater/Documents/2021_strips_soil_column/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE349893-0517-9648-817E-0A6E6082F87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365ADDB8-2EEF-DD49-B45C-BA2EE7409674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16640" activeTab="3" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Rainfall 1" sheetId="1" r:id="rId1"/>
     <sheet name="Rainfall 2" sheetId="2" r:id="rId2"/>
     <sheet name="Rainfall 3" sheetId="3" r:id="rId3"/>
     <sheet name="Rainfall 4" sheetId="4" r:id="rId4"/>
-    <sheet name="Rainfall 5" sheetId="5" r:id="rId5"/>
-    <sheet name="Rainfall 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -46,10 +35,19 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{98B61FB3-52CC-9F41-BC50-21752F5C5A25}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Please make unique name, not start with number, add project name</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -64,10 +62,19 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{6AB049BB-9B62-234E-B092-DC3406986DB0}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Please make unique name, not start with number, add project name</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -82,10 +89,19 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{944BE181-8429-0C41-98F4-DAD1FFAEEFEF}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Please make unique name, not start with number, add project name</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -93,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="449">
   <si>
     <t>unique sample_id</t>
   </si>
@@ -1534,7 +1550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1546,6 +1562,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1890,28 +1908,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A39224-C7A3-DC45-833D-204FCB526563}">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C55"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1925,37 +1943,40 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>340</v>
+      </c>
+      <c r="F1" t="s">
         <v>52</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>118</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>228</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>229</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>119</v>
       </c>
@@ -1969,25 +1990,22 @@
         <v>20210531</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>1500</v>
       </c>
-      <c r="F2" t="s">
-        <v>227</v>
-      </c>
-      <c r="G2" t="s">
-        <v>227</v>
-      </c>
-      <c r="H2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I2" s="3">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="3">
         <v>20210603</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K2" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>120</v>
       </c>
@@ -2001,25 +2019,22 @@
         <v>20210531</v>
       </c>
       <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>3000</v>
       </c>
-      <c r="F3" t="s">
-        <v>227</v>
-      </c>
-      <c r="G3" t="s">
-        <v>227</v>
-      </c>
-      <c r="H3" t="s">
-        <v>227</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="3">
         <v>20210603</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K3" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>121</v>
       </c>
@@ -2033,25 +2048,22 @@
         <v>20210531</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <v>1500</v>
       </c>
-      <c r="F4" t="s">
-        <v>227</v>
-      </c>
-      <c r="G4" t="s">
-        <v>227</v>
-      </c>
-      <c r="H4" t="s">
-        <v>227</v>
-      </c>
-      <c r="I4" s="3">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="3">
         <v>20210603</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K4" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>122</v>
       </c>
@@ -2065,25 +2077,22 @@
         <v>20210531</v>
       </c>
       <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>3000</v>
       </c>
-      <c r="F5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G5" t="s">
-        <v>227</v>
-      </c>
-      <c r="H5" t="s">
-        <v>227</v>
-      </c>
-      <c r="I5" s="3">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="3">
         <v>20210604</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K5" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>123</v>
       </c>
@@ -2097,25 +2106,22 @@
         <v>20210531</v>
       </c>
       <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>1500</v>
       </c>
-      <c r="F6" t="s">
-        <v>227</v>
-      </c>
-      <c r="G6" t="s">
-        <v>227</v>
-      </c>
-      <c r="H6" t="s">
-        <v>227</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="3">
         <v>20210603</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K6" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
@@ -2129,25 +2135,22 @@
         <v>20210531</v>
       </c>
       <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>3000</v>
       </c>
-      <c r="F7" t="s">
-        <v>227</v>
-      </c>
-      <c r="G7" t="s">
-        <v>227</v>
-      </c>
-      <c r="H7" t="s">
-        <v>227</v>
-      </c>
-      <c r="I7" s="3">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="3">
         <v>20210604</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K7" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>125</v>
       </c>
@@ -2161,25 +2164,22 @@
         <v>20210531</v>
       </c>
       <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
         <v>1500</v>
       </c>
-      <c r="F8" t="s">
-        <v>227</v>
-      </c>
-      <c r="G8" t="s">
-        <v>227</v>
-      </c>
-      <c r="H8" t="s">
-        <v>227</v>
-      </c>
-      <c r="I8" s="3">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="3">
         <v>20210604</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K8" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -2193,25 +2193,22 @@
         <v>20210531</v>
       </c>
       <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
         <v>3000</v>
       </c>
-      <c r="F9" t="s">
-        <v>227</v>
-      </c>
-      <c r="G9" t="s">
-        <v>227</v>
-      </c>
-      <c r="H9" t="s">
-        <v>227</v>
-      </c>
-      <c r="I9" s="3">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="3">
         <v>20210603</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K9" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>127</v>
       </c>
@@ -2225,25 +2222,22 @@
         <v>20210531</v>
       </c>
       <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>1500</v>
       </c>
-      <c r="F10" t="s">
-        <v>227</v>
-      </c>
-      <c r="G10" t="s">
-        <v>227</v>
-      </c>
-      <c r="H10" t="s">
-        <v>227</v>
-      </c>
-      <c r="I10" s="3">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="3">
         <v>20210603</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K10" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>128</v>
       </c>
@@ -2257,25 +2251,22 @@
         <v>20210531</v>
       </c>
       <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
         <v>3000</v>
       </c>
-      <c r="F11" t="s">
-        <v>227</v>
-      </c>
-      <c r="G11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H11" t="s">
-        <v>227</v>
-      </c>
-      <c r="I11" s="3">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="3">
         <v>20210605</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K11" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>129</v>
       </c>
@@ -2289,25 +2280,22 @@
         <v>20210531</v>
       </c>
       <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
         <v>1500</v>
       </c>
-      <c r="F12" t="s">
-        <v>227</v>
-      </c>
-      <c r="G12" t="s">
-        <v>227</v>
-      </c>
-      <c r="H12" t="s">
-        <v>227</v>
-      </c>
-      <c r="I12" s="3">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="3">
         <v>20210604</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K12" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>130</v>
       </c>
@@ -2321,25 +2309,22 @@
         <v>20210531</v>
       </c>
       <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
         <v>3000</v>
       </c>
-      <c r="F13" t="s">
-        <v>227</v>
-      </c>
-      <c r="G13" t="s">
-        <v>227</v>
-      </c>
-      <c r="H13" t="s">
-        <v>227</v>
-      </c>
-      <c r="I13" s="3">
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="3">
         <v>20210604</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K13" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>131</v>
       </c>
@@ -2353,25 +2338,22 @@
         <v>20210531</v>
       </c>
       <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
         <v>1500</v>
       </c>
-      <c r="F14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G14" t="s">
-        <v>227</v>
-      </c>
-      <c r="H14" t="s">
-        <v>227</v>
-      </c>
-      <c r="I14" s="3">
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="3">
         <v>20210604</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K14" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>132</v>
       </c>
@@ -2385,25 +2367,22 @@
         <v>20210531</v>
       </c>
       <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
         <v>3000</v>
       </c>
-      <c r="F15" t="s">
-        <v>227</v>
-      </c>
-      <c r="G15" t="s">
-        <v>227</v>
-      </c>
-      <c r="H15" t="s">
-        <v>227</v>
-      </c>
-      <c r="I15" s="3">
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="3">
         <v>20210604</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K15" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>133</v>
       </c>
@@ -2417,25 +2396,22 @@
         <v>20210531</v>
       </c>
       <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
         <v>1500</v>
       </c>
-      <c r="F16" t="s">
-        <v>227</v>
-      </c>
-      <c r="G16" t="s">
-        <v>227</v>
-      </c>
-      <c r="H16" t="s">
-        <v>227</v>
-      </c>
-      <c r="I16" s="3">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="3">
         <v>20210603</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>134</v>
       </c>
@@ -2449,25 +2425,22 @@
         <v>20210531</v>
       </c>
       <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
         <v>3000</v>
       </c>
-      <c r="F17" t="s">
-        <v>227</v>
-      </c>
-      <c r="G17" t="s">
-        <v>227</v>
-      </c>
-      <c r="H17" t="s">
-        <v>227</v>
-      </c>
-      <c r="I17" s="3">
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="3">
         <v>20210603</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>135</v>
       </c>
@@ -2481,25 +2454,22 @@
         <v>20210531</v>
       </c>
       <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
         <v>1500</v>
       </c>
-      <c r="F18" t="s">
-        <v>227</v>
-      </c>
-      <c r="G18" t="s">
-        <v>227</v>
-      </c>
-      <c r="H18" t="s">
-        <v>227</v>
-      </c>
-      <c r="I18" s="3">
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="3">
         <v>20210604</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>136</v>
       </c>
@@ -2513,25 +2483,22 @@
         <v>20210531</v>
       </c>
       <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
         <v>3000</v>
       </c>
-      <c r="F19" t="s">
-        <v>227</v>
-      </c>
-      <c r="G19" t="s">
-        <v>227</v>
-      </c>
-      <c r="H19" t="s">
-        <v>227</v>
-      </c>
-      <c r="I19" s="3">
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="3">
         <v>20210604</v>
       </c>
-      <c r="J19" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>137</v>
       </c>
@@ -2545,25 +2512,22 @@
         <v>20210602</v>
       </c>
       <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
         <v>1500</v>
       </c>
-      <c r="F20" t="s">
-        <v>227</v>
-      </c>
-      <c r="G20" t="s">
-        <v>227</v>
-      </c>
-      <c r="H20" t="s">
-        <v>227</v>
-      </c>
-      <c r="I20" s="3">
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="3">
         <v>20210605</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>138</v>
       </c>
@@ -2577,25 +2541,22 @@
         <v>20210602</v>
       </c>
       <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
         <v>3000</v>
       </c>
-      <c r="F21" t="s">
-        <v>227</v>
-      </c>
-      <c r="G21" t="s">
-        <v>227</v>
-      </c>
-      <c r="H21" t="s">
-        <v>227</v>
-      </c>
-      <c r="I21" s="3">
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="3">
         <v>20210605</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>139</v>
       </c>
@@ -2609,25 +2570,22 @@
         <v>20210602</v>
       </c>
       <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
         <v>1500</v>
       </c>
-      <c r="F22" t="s">
-        <v>227</v>
-      </c>
-      <c r="G22" t="s">
-        <v>227</v>
-      </c>
-      <c r="H22" t="s">
-        <v>227</v>
-      </c>
-      <c r="I22" s="3">
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="3">
         <v>20210605</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>140</v>
       </c>
@@ -2641,25 +2599,22 @@
         <v>20210602</v>
       </c>
       <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
         <v>3000</v>
       </c>
-      <c r="F23" t="s">
-        <v>227</v>
-      </c>
-      <c r="G23" t="s">
-        <v>227</v>
-      </c>
-      <c r="H23" t="s">
-        <v>227</v>
-      </c>
-      <c r="I23" s="3">
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="3">
         <v>20210605</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>141</v>
       </c>
@@ -2673,25 +2628,22 @@
         <v>20210602</v>
       </c>
       <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
         <v>1500</v>
       </c>
-      <c r="F24" t="s">
-        <v>227</v>
-      </c>
-      <c r="G24" t="s">
-        <v>227</v>
-      </c>
-      <c r="H24" t="s">
-        <v>227</v>
-      </c>
-      <c r="I24" s="3">
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="3">
         <v>20210605</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>142</v>
       </c>
@@ -2705,25 +2657,22 @@
         <v>20210602</v>
       </c>
       <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
         <v>3000</v>
       </c>
-      <c r="F25" t="s">
-        <v>227</v>
-      </c>
-      <c r="G25" t="s">
-        <v>227</v>
-      </c>
-      <c r="H25" t="s">
-        <v>227</v>
-      </c>
-      <c r="I25" s="3">
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="3">
         <v>20210605</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>143</v>
       </c>
@@ -2737,25 +2686,22 @@
         <v>20210602</v>
       </c>
       <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
         <v>1500</v>
       </c>
-      <c r="F26" t="s">
-        <v>227</v>
-      </c>
-      <c r="G26" t="s">
-        <v>227</v>
-      </c>
-      <c r="H26" t="s">
-        <v>227</v>
-      </c>
-      <c r="I26" s="3">
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="3">
         <v>20210605</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>144</v>
       </c>
@@ -2769,25 +2715,22 @@
         <v>20210602</v>
       </c>
       <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
         <v>3000</v>
       </c>
-      <c r="F27" t="s">
-        <v>227</v>
-      </c>
-      <c r="G27" t="s">
-        <v>227</v>
-      </c>
-      <c r="H27" t="s">
-        <v>227</v>
-      </c>
-      <c r="I27" s="3">
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="3">
         <v>20210605</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>145</v>
       </c>
@@ -2801,25 +2744,22 @@
         <v>20210602</v>
       </c>
       <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
         <v>1500</v>
       </c>
-      <c r="F28" t="s">
-        <v>227</v>
-      </c>
-      <c r="G28" t="s">
-        <v>227</v>
-      </c>
-      <c r="H28" t="s">
-        <v>227</v>
-      </c>
-      <c r="I28" s="3">
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="3">
         <v>20210605</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>146</v>
       </c>
@@ -2833,25 +2773,22 @@
         <v>20210602</v>
       </c>
       <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
         <v>3000</v>
       </c>
-      <c r="F29" t="s">
-        <v>227</v>
-      </c>
-      <c r="G29" t="s">
-        <v>227</v>
-      </c>
-      <c r="H29" t="s">
-        <v>227</v>
-      </c>
-      <c r="I29" s="3">
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="3">
         <v>20210605</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>147</v>
       </c>
@@ -2865,25 +2802,22 @@
         <v>20210602</v>
       </c>
       <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
         <v>1500</v>
       </c>
-      <c r="F30" t="s">
-        <v>227</v>
-      </c>
-      <c r="G30" t="s">
-        <v>227</v>
-      </c>
-      <c r="H30" t="s">
-        <v>227</v>
-      </c>
-      <c r="I30" s="3">
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="3">
         <v>20210605</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>148</v>
       </c>
@@ -2897,25 +2831,22 @@
         <v>20210602</v>
       </c>
       <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
         <v>3000</v>
       </c>
-      <c r="F31" t="s">
-        <v>227</v>
-      </c>
-      <c r="G31" t="s">
-        <v>227</v>
-      </c>
-      <c r="H31" t="s">
-        <v>227</v>
-      </c>
-      <c r="I31" s="3">
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="3">
         <v>20210605</v>
       </c>
-      <c r="J31" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>149</v>
       </c>
@@ -2929,25 +2860,22 @@
         <v>20210602</v>
       </c>
       <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
         <v>1500</v>
       </c>
-      <c r="F32" t="s">
-        <v>227</v>
-      </c>
-      <c r="G32" t="s">
-        <v>227</v>
-      </c>
-      <c r="H32" t="s">
-        <v>227</v>
-      </c>
-      <c r="I32" s="3">
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="3">
         <v>20210605</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>150</v>
       </c>
@@ -2961,25 +2889,22 @@
         <v>20210602</v>
       </c>
       <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
         <v>3000</v>
       </c>
-      <c r="F33" t="s">
-        <v>227</v>
-      </c>
-      <c r="G33" t="s">
-        <v>227</v>
-      </c>
-      <c r="H33" t="s">
-        <v>227</v>
-      </c>
-      <c r="I33" s="3">
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="3">
         <v>20210605</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>151</v>
       </c>
@@ -2993,25 +2918,22 @@
         <v>20210602</v>
       </c>
       <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
         <v>1500</v>
       </c>
-      <c r="F34" t="s">
-        <v>227</v>
-      </c>
-      <c r="G34" t="s">
-        <v>227</v>
-      </c>
-      <c r="H34" t="s">
-        <v>227</v>
-      </c>
-      <c r="I34" s="3">
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="3">
         <v>20210605</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>152</v>
       </c>
@@ -3025,25 +2947,22 @@
         <v>20210602</v>
       </c>
       <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
         <v>3000</v>
       </c>
-      <c r="F35" t="s">
-        <v>227</v>
-      </c>
-      <c r="G35" t="s">
-        <v>227</v>
-      </c>
-      <c r="H35" t="s">
-        <v>227</v>
-      </c>
-      <c r="I35" s="3">
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="3">
         <v>20210605</v>
       </c>
-      <c r="J35" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>153</v>
       </c>
@@ -3057,25 +2976,22 @@
         <v>20210602</v>
       </c>
       <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
         <v>1500</v>
       </c>
-      <c r="F36" t="s">
-        <v>227</v>
-      </c>
-      <c r="G36" t="s">
-        <v>227</v>
-      </c>
-      <c r="H36" t="s">
-        <v>227</v>
-      </c>
-      <c r="I36" s="3">
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="3">
         <v>20210605</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>154</v>
       </c>
@@ -3089,25 +3005,22 @@
         <v>20210602</v>
       </c>
       <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
         <v>3000</v>
       </c>
-      <c r="F37" t="s">
-        <v>227</v>
-      </c>
-      <c r="G37" t="s">
-        <v>227</v>
-      </c>
-      <c r="H37" t="s">
-        <v>227</v>
-      </c>
-      <c r="I37" s="3">
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="3">
         <v>20210605</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>155</v>
       </c>
@@ -3121,25 +3034,22 @@
         <v>20210604</v>
       </c>
       <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
         <v>1500</v>
       </c>
-      <c r="F38" t="s">
-        <v>227</v>
-      </c>
-      <c r="G38" t="s">
-        <v>227</v>
-      </c>
-      <c r="H38" t="s">
-        <v>227</v>
-      </c>
-      <c r="I38" s="3">
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="3">
         <v>20210606</v>
       </c>
-      <c r="J38" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>156</v>
       </c>
@@ -3153,25 +3063,22 @@
         <v>20210604</v>
       </c>
       <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
         <v>3000</v>
       </c>
-      <c r="F39" t="s">
-        <v>227</v>
-      </c>
-      <c r="G39" t="s">
-        <v>227</v>
-      </c>
-      <c r="H39" t="s">
-        <v>227</v>
-      </c>
-      <c r="I39" s="3">
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="3">
         <v>20210606</v>
       </c>
-      <c r="J39" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>157</v>
       </c>
@@ -3185,25 +3092,22 @@
         <v>20210604</v>
       </c>
       <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
         <v>1500</v>
       </c>
-      <c r="F40" t="s">
-        <v>227</v>
-      </c>
-      <c r="G40" t="s">
-        <v>227</v>
-      </c>
-      <c r="H40" t="s">
-        <v>227</v>
-      </c>
-      <c r="I40" s="3">
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="3">
         <v>20210606</v>
       </c>
-      <c r="J40" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>158</v>
       </c>
@@ -3217,25 +3121,22 @@
         <v>20210604</v>
       </c>
       <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
         <v>3000</v>
       </c>
-      <c r="F41" t="s">
-        <v>227</v>
-      </c>
-      <c r="G41" t="s">
-        <v>227</v>
-      </c>
-      <c r="H41" t="s">
-        <v>227</v>
-      </c>
-      <c r="I41" s="3">
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="3">
         <v>20210606</v>
       </c>
-      <c r="J41" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>159</v>
       </c>
@@ -3249,25 +3150,22 @@
         <v>20210604</v>
       </c>
       <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
         <v>1500</v>
       </c>
-      <c r="F42" t="s">
-        <v>227</v>
-      </c>
-      <c r="G42" t="s">
-        <v>227</v>
-      </c>
-      <c r="H42" t="s">
-        <v>227</v>
-      </c>
-      <c r="I42" s="3">
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="3">
         <v>20210606</v>
       </c>
-      <c r="J42" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>160</v>
       </c>
@@ -3281,25 +3179,22 @@
         <v>20210604</v>
       </c>
       <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
         <v>3000</v>
       </c>
-      <c r="F43" t="s">
-        <v>227</v>
-      </c>
-      <c r="G43" t="s">
-        <v>227</v>
-      </c>
-      <c r="H43" t="s">
-        <v>227</v>
-      </c>
-      <c r="I43" s="3">
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="3">
         <v>20210606</v>
       </c>
-      <c r="J43" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>161</v>
       </c>
@@ -3313,25 +3208,22 @@
         <v>20210604</v>
       </c>
       <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
         <v>1500</v>
       </c>
-      <c r="F44" t="s">
-        <v>227</v>
-      </c>
-      <c r="G44" t="s">
-        <v>227</v>
-      </c>
-      <c r="H44" t="s">
-        <v>227</v>
-      </c>
-      <c r="I44" s="3">
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="3">
         <v>20210606</v>
       </c>
-      <c r="J44" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>162</v>
       </c>
@@ -3345,25 +3237,22 @@
         <v>20210604</v>
       </c>
       <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
         <v>3000</v>
       </c>
-      <c r="F45" t="s">
-        <v>227</v>
-      </c>
-      <c r="G45" t="s">
-        <v>227</v>
-      </c>
-      <c r="H45" t="s">
-        <v>227</v>
-      </c>
-      <c r="I45" s="3">
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="3">
         <v>20210606</v>
       </c>
-      <c r="J45" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>163</v>
       </c>
@@ -3377,25 +3266,22 @@
         <v>20210604</v>
       </c>
       <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
         <v>1500</v>
       </c>
-      <c r="F46" t="s">
-        <v>227</v>
-      </c>
-      <c r="G46" t="s">
-        <v>227</v>
-      </c>
-      <c r="H46" t="s">
-        <v>227</v>
-      </c>
-      <c r="I46" s="3">
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="3">
         <v>20210606</v>
       </c>
-      <c r="J46" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>164</v>
       </c>
@@ -3409,25 +3295,22 @@
         <v>20210604</v>
       </c>
       <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
         <v>3000</v>
       </c>
-      <c r="F47" t="s">
-        <v>227</v>
-      </c>
-      <c r="G47" t="s">
-        <v>227</v>
-      </c>
-      <c r="H47" t="s">
-        <v>227</v>
-      </c>
-      <c r="I47" s="3">
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="3">
         <v>20210606</v>
       </c>
-      <c r="J47" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>165</v>
       </c>
@@ -3441,25 +3324,22 @@
         <v>20210604</v>
       </c>
       <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
         <v>1500</v>
       </c>
-      <c r="F48" t="s">
-        <v>227</v>
-      </c>
-      <c r="G48" t="s">
-        <v>227</v>
-      </c>
-      <c r="H48" t="s">
-        <v>227</v>
-      </c>
-      <c r="I48" s="3">
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="3">
         <v>20210607</v>
       </c>
-      <c r="J48" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>166</v>
       </c>
@@ -3473,25 +3353,22 @@
         <v>20210604</v>
       </c>
       <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
         <v>3000</v>
       </c>
-      <c r="F49" t="s">
-        <v>227</v>
-      </c>
-      <c r="G49" t="s">
-        <v>227</v>
-      </c>
-      <c r="H49" t="s">
-        <v>227</v>
-      </c>
-      <c r="I49" s="3">
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="3">
         <v>20210607</v>
       </c>
-      <c r="J49" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>167</v>
       </c>
@@ -3505,25 +3382,22 @@
         <v>20210604</v>
       </c>
       <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
         <v>1500</v>
       </c>
-      <c r="F50" t="s">
-        <v>227</v>
-      </c>
-      <c r="G50" t="s">
-        <v>227</v>
-      </c>
-      <c r="H50" t="s">
-        <v>227</v>
-      </c>
-      <c r="I50" s="3">
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="3">
         <v>20210607</v>
       </c>
-      <c r="J50" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>168</v>
       </c>
@@ -3537,25 +3411,22 @@
         <v>20210604</v>
       </c>
       <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
         <v>3000</v>
       </c>
-      <c r="F51" t="s">
-        <v>227</v>
-      </c>
-      <c r="G51" t="s">
-        <v>227</v>
-      </c>
-      <c r="H51" t="s">
-        <v>227</v>
-      </c>
-      <c r="I51" s="3">
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="3">
         <v>20210606</v>
       </c>
-      <c r="J51" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>169</v>
       </c>
@@ -3569,25 +3440,22 @@
         <v>20210604</v>
       </c>
       <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
         <v>1500</v>
       </c>
-      <c r="F52" t="s">
-        <v>227</v>
-      </c>
-      <c r="G52" t="s">
-        <v>227</v>
-      </c>
-      <c r="H52" t="s">
-        <v>227</v>
-      </c>
-      <c r="I52" s="3">
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="3">
         <v>20210607</v>
       </c>
-      <c r="J52" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>170</v>
       </c>
@@ -3601,25 +3469,22 @@
         <v>20210604</v>
       </c>
       <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
         <v>3000</v>
       </c>
-      <c r="F53" t="s">
-        <v>227</v>
-      </c>
-      <c r="G53" t="s">
-        <v>227</v>
-      </c>
-      <c r="H53" t="s">
-        <v>227</v>
-      </c>
-      <c r="I53" s="3">
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="3">
         <v>20210607</v>
       </c>
-      <c r="J53" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K53" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>171</v>
       </c>
@@ -3633,25 +3498,22 @@
         <v>20210604</v>
       </c>
       <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
         <v>1500</v>
       </c>
-      <c r="F54" t="s">
-        <v>227</v>
-      </c>
-      <c r="G54" t="s">
-        <v>227</v>
-      </c>
-      <c r="H54" t="s">
-        <v>227</v>
-      </c>
-      <c r="I54" s="3">
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="3">
         <v>20210607</v>
       </c>
-      <c r="J54" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K54" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>172</v>
       </c>
@@ -3665,21 +3527,18 @@
         <v>20210604</v>
       </c>
       <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
         <v>3000</v>
       </c>
-      <c r="F55" t="s">
-        <v>227</v>
-      </c>
-      <c r="G55" t="s">
-        <v>227</v>
-      </c>
-      <c r="H55" t="s">
-        <v>227</v>
-      </c>
-      <c r="I55" s="3">
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="3">
         <v>20210606</v>
       </c>
-      <c r="J55" s="2" t="s">
+      <c r="K55" s="2" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3695,7 +3554,7 @@
   <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7744,8 +7603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556C630F-CED0-3C49-9F7A-3D77E458B865}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9251,7 +9110,7 @@
         <v>322</v>
       </c>
       <c r="D38" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E38" s="2">
         <v>4</v>
@@ -9260,17 +9119,15 @@
         <v>1000</v>
       </c>
       <c r="G38" s="8">
-        <v>100</v>
-      </c>
-      <c r="H38" s="8">
-        <v>1000</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="H38" s="8"/>
       <c r="I38" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-104</v>
       </c>
       <c r="J38" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>230</v>
@@ -9291,7 +9148,7 @@
         <v>323</v>
       </c>
       <c r="D39" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E39" s="2">
         <v>4</v>
@@ -9300,17 +9157,15 @@
         <v>1000</v>
       </c>
       <c r="G39" s="8">
-        <v>100</v>
-      </c>
-      <c r="H39" s="8">
-        <v>1000</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="H39" s="8"/>
       <c r="I39" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-89</v>
       </c>
       <c r="J39" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>230</v>
@@ -9331,7 +9186,7 @@
         <v>324</v>
       </c>
       <c r="D40" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E40" s="2">
         <v>4</v>
@@ -9340,17 +9195,15 @@
         <v>1000</v>
       </c>
       <c r="G40" s="8">
-        <v>100</v>
-      </c>
-      <c r="H40" s="8">
-        <v>1000</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H40" s="8"/>
       <c r="I40" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-88</v>
       </c>
       <c r="J40" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>230</v>
@@ -9371,7 +9224,7 @@
         <v>325</v>
       </c>
       <c r="D41" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E41" s="2">
         <v>4</v>
@@ -9380,17 +9233,15 @@
         <v>1000</v>
       </c>
       <c r="G41" s="8">
-        <v>100</v>
-      </c>
-      <c r="H41" s="8">
-        <v>1000</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H41" s="8"/>
       <c r="I41" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-88</v>
       </c>
       <c r="J41" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>230</v>
@@ -9411,7 +9262,7 @@
         <v>326</v>
       </c>
       <c r="D42" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E42" s="2">
         <v>4</v>
@@ -9420,17 +9271,15 @@
         <v>1000</v>
       </c>
       <c r="G42" s="8">
-        <v>100</v>
-      </c>
-      <c r="H42" s="8">
-        <v>1000</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H42" s="8"/>
       <c r="I42" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-88</v>
       </c>
       <c r="J42" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>230</v>
@@ -9451,7 +9300,7 @@
         <v>327</v>
       </c>
       <c r="D43" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E43" s="2">
         <v>4</v>
@@ -9460,17 +9309,15 @@
         <v>1000</v>
       </c>
       <c r="G43" s="8">
-        <v>100</v>
-      </c>
-      <c r="H43" s="8">
-        <v>1000</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="H43" s="8"/>
       <c r="I43" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-89</v>
       </c>
       <c r="J43" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>230</v>
@@ -9491,7 +9338,7 @@
         <v>328</v>
       </c>
       <c r="D44" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E44" s="2">
         <v>4</v>
@@ -9500,17 +9347,15 @@
         <v>1000</v>
       </c>
       <c r="G44" s="8">
-        <v>100</v>
-      </c>
-      <c r="H44" s="8">
-        <v>1000</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H44" s="8"/>
       <c r="I44" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-88</v>
       </c>
       <c r="J44" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>230</v>
@@ -9531,7 +9376,7 @@
         <v>329</v>
       </c>
       <c r="D45" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E45" s="2">
         <v>4</v>
@@ -9540,17 +9385,15 @@
         <v>1000</v>
       </c>
       <c r="G45" s="8">
-        <v>100</v>
-      </c>
-      <c r="H45" s="8">
-        <v>1000</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H45" s="8"/>
       <c r="I45" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-88</v>
       </c>
       <c r="J45" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>230</v>
@@ -9571,7 +9414,7 @@
         <v>330</v>
       </c>
       <c r="D46" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E46" s="2">
         <v>4</v>
@@ -9580,17 +9423,15 @@
         <v>1000</v>
       </c>
       <c r="G46" s="8">
-        <v>100</v>
-      </c>
-      <c r="H46" s="8">
-        <v>1000</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H46" s="8"/>
       <c r="I46" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-88</v>
       </c>
       <c r="J46" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>230</v>
@@ -9611,7 +9452,7 @@
         <v>331</v>
       </c>
       <c r="D47" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E47" s="2">
         <v>4</v>
@@ -9620,17 +9461,15 @@
         <v>1000</v>
       </c>
       <c r="G47" s="8">
-        <v>100</v>
-      </c>
-      <c r="H47" s="8">
-        <v>1000</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H47" s="8"/>
       <c r="I47" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-88</v>
       </c>
       <c r="J47" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>230</v>
@@ -9651,7 +9490,7 @@
         <v>332</v>
       </c>
       <c r="D48" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E48" s="2">
         <v>4</v>
@@ -9660,17 +9499,15 @@
         <v>1000</v>
       </c>
       <c r="G48" s="8">
-        <v>100</v>
-      </c>
-      <c r="H48" s="8">
-        <v>1000</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="H48" s="8"/>
       <c r="I48" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-89</v>
       </c>
       <c r="J48" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>230</v>
@@ -9691,7 +9528,7 @@
         <v>333</v>
       </c>
       <c r="D49" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E49" s="2">
         <v>4</v>
@@ -9700,17 +9537,15 @@
         <v>1000</v>
       </c>
       <c r="G49" s="8">
-        <v>100</v>
-      </c>
-      <c r="H49" s="8">
-        <v>1000</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="H49" s="8"/>
       <c r="I49" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-103</v>
       </c>
       <c r="J49" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>230</v>
@@ -9731,7 +9566,7 @@
         <v>334</v>
       </c>
       <c r="D50" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E50" s="2">
         <v>4</v>
@@ -9740,17 +9575,15 @@
         <v>1000</v>
       </c>
       <c r="G50" s="8">
-        <v>100</v>
-      </c>
-      <c r="H50" s="8">
-        <v>1000</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="H50" s="8"/>
       <c r="I50" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-89</v>
       </c>
       <c r="J50" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>230</v>
@@ -9771,7 +9604,7 @@
         <v>335</v>
       </c>
       <c r="D51" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E51" s="2">
         <v>4</v>
@@ -9780,17 +9613,15 @@
         <v>1000</v>
       </c>
       <c r="G51" s="8">
-        <v>100</v>
-      </c>
-      <c r="H51" s="8">
-        <v>1000</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="H51" s="8"/>
       <c r="I51" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-89</v>
       </c>
       <c r="J51" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>230</v>
@@ -9811,7 +9642,7 @@
         <v>336</v>
       </c>
       <c r="D52" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E52" s="2">
         <v>4</v>
@@ -9820,17 +9651,15 @@
         <v>1000</v>
       </c>
       <c r="G52" s="8">
-        <v>100</v>
-      </c>
-      <c r="H52" s="8">
-        <v>1000</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H52" s="8"/>
       <c r="I52" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-88</v>
       </c>
       <c r="J52" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K52" s="2" t="s">
         <v>230</v>
@@ -9851,7 +9680,7 @@
         <v>337</v>
       </c>
       <c r="D53" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E53" s="2">
         <v>4</v>
@@ -9860,17 +9689,15 @@
         <v>1000</v>
       </c>
       <c r="G53" s="8">
-        <v>100</v>
-      </c>
-      <c r="H53" s="8">
-        <v>1000</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H53" s="8"/>
       <c r="I53" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-88</v>
       </c>
       <c r="J53" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>230</v>
@@ -9891,7 +9718,7 @@
         <v>338</v>
       </c>
       <c r="D54" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E54" s="2">
         <v>4</v>
@@ -9900,17 +9727,15 @@
         <v>1000</v>
       </c>
       <c r="G54" s="8">
-        <v>100</v>
-      </c>
-      <c r="H54" s="8">
-        <v>1000</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="H54" s="8"/>
       <c r="I54" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-89</v>
       </c>
       <c r="J54" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>230</v>
@@ -9931,7 +9756,7 @@
         <v>339</v>
       </c>
       <c r="D55" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E55" s="2">
         <v>4</v>
@@ -9940,17 +9765,15 @@
         <v>1000</v>
       </c>
       <c r="G55" s="8">
-        <v>100</v>
-      </c>
-      <c r="H55" s="8">
-        <v>1000</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H55" s="8"/>
       <c r="I55" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>-88</v>
       </c>
       <c r="J55" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>230</v>
@@ -9964,28 +9787,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C5F78B-ED0A-A94A-92EC-0E12CA5D830D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C14A820-FA44-D343-8D24-028C09F8EE09}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update with volume from B3 R4
</commit_message>
<xml_diff>
--- a/Data/LeachateData.xlsx
+++ b/Data/LeachateData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredflater/Documents/2021_strips_soil_column/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365ADDB8-2EEF-DD49-B45C-BA2EE7409674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C19922D-1279-6144-A60E-6190F014019D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16640" activeTab="3" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
   </bookViews>
@@ -7604,7 +7604,7 @@
   <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="Q52" sqref="Q52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9121,10 +9121,12 @@
       <c r="G38" s="8">
         <v>104</v>
       </c>
-      <c r="H38" s="8"/>
+      <c r="H38" s="8">
+        <v>827</v>
+      </c>
       <c r="I38" s="2">
         <f t="shared" si="0"/>
-        <v>-104</v>
+        <v>723</v>
       </c>
       <c r="J38" s="2">
         <v>20210625</v>
@@ -9159,10 +9161,12 @@
       <c r="G39" s="8">
         <v>89</v>
       </c>
-      <c r="H39" s="8"/>
+      <c r="H39" s="8">
+        <v>827</v>
+      </c>
       <c r="I39" s="2">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>738</v>
       </c>
       <c r="J39" s="2">
         <v>20210625</v>
@@ -9197,10 +9201,12 @@
       <c r="G40" s="8">
         <v>88</v>
       </c>
-      <c r="H40" s="8"/>
+      <c r="H40" s="8">
+        <v>893</v>
+      </c>
       <c r="I40" s="2">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>805</v>
       </c>
       <c r="J40" s="2">
         <v>20210625</v>
@@ -9235,10 +9241,12 @@
       <c r="G41" s="8">
         <v>88</v>
       </c>
-      <c r="H41" s="8"/>
+      <c r="H41" s="8">
+        <v>856</v>
+      </c>
       <c r="I41" s="2">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>768</v>
       </c>
       <c r="J41" s="2">
         <v>20210625</v>
@@ -9273,10 +9281,12 @@
       <c r="G42" s="8">
         <v>88</v>
       </c>
-      <c r="H42" s="8"/>
+      <c r="H42" s="8">
+        <v>817</v>
+      </c>
       <c r="I42" s="2">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>729</v>
       </c>
       <c r="J42" s="2">
         <v>20210625</v>
@@ -9311,10 +9321,12 @@
       <c r="G43" s="8">
         <v>89</v>
       </c>
-      <c r="H43" s="8"/>
+      <c r="H43" s="8">
+        <v>817</v>
+      </c>
       <c r="I43" s="2">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>728</v>
       </c>
       <c r="J43" s="2">
         <v>20210625</v>
@@ -9349,10 +9361,12 @@
       <c r="G44" s="8">
         <v>88</v>
       </c>
-      <c r="H44" s="8"/>
+      <c r="H44" s="8">
+        <v>896</v>
+      </c>
       <c r="I44" s="2">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>808</v>
       </c>
       <c r="J44" s="2">
         <v>20210625</v>
@@ -9387,10 +9401,12 @@
       <c r="G45" s="8">
         <v>88</v>
       </c>
-      <c r="H45" s="8"/>
+      <c r="H45" s="8">
+        <v>808</v>
+      </c>
       <c r="I45" s="2">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>720</v>
       </c>
       <c r="J45" s="2">
         <v>20210625</v>
@@ -9425,10 +9441,12 @@
       <c r="G46" s="8">
         <v>88</v>
       </c>
-      <c r="H46" s="8"/>
+      <c r="H46" s="8">
+        <v>808</v>
+      </c>
       <c r="I46" s="2">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>720</v>
       </c>
       <c r="J46" s="2">
         <v>20210625</v>
@@ -9463,10 +9481,12 @@
       <c r="G47" s="8">
         <v>88</v>
       </c>
-      <c r="H47" s="8"/>
+      <c r="H47" s="8">
+        <v>846</v>
+      </c>
       <c r="I47" s="2">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>758</v>
       </c>
       <c r="J47" s="2">
         <v>20210625</v>
@@ -9501,10 +9521,12 @@
       <c r="G48" s="8">
         <v>89</v>
       </c>
-      <c r="H48" s="8"/>
+      <c r="H48" s="8">
+        <v>903</v>
+      </c>
       <c r="I48" s="2">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>814</v>
       </c>
       <c r="J48" s="2">
         <v>20210625</v>
@@ -9539,10 +9561,12 @@
       <c r="G49" s="8">
         <v>103</v>
       </c>
-      <c r="H49" s="8"/>
+      <c r="H49" s="8">
+        <v>868</v>
+      </c>
       <c r="I49" s="2">
         <f t="shared" si="0"/>
-        <v>-103</v>
+        <v>765</v>
       </c>
       <c r="J49" s="2">
         <v>20210625</v>
@@ -9577,10 +9601,12 @@
       <c r="G50" s="8">
         <v>89</v>
       </c>
-      <c r="H50" s="8"/>
+      <c r="H50" s="8">
+        <v>915</v>
+      </c>
       <c r="I50" s="2">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>826</v>
       </c>
       <c r="J50" s="2">
         <v>20210625</v>
@@ -9615,10 +9641,12 @@
       <c r="G51" s="8">
         <v>89</v>
       </c>
-      <c r="H51" s="8"/>
+      <c r="H51" s="8">
+        <v>863</v>
+      </c>
       <c r="I51" s="2">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>774</v>
       </c>
       <c r="J51" s="2">
         <v>20210625</v>
@@ -9653,10 +9681,12 @@
       <c r="G52" s="8">
         <v>88</v>
       </c>
-      <c r="H52" s="8"/>
+      <c r="H52" s="8">
+        <v>878</v>
+      </c>
       <c r="I52" s="2">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>790</v>
       </c>
       <c r="J52" s="2">
         <v>20210625</v>
@@ -9691,10 +9721,12 @@
       <c r="G53" s="8">
         <v>88</v>
       </c>
-      <c r="H53" s="8"/>
+      <c r="H53" s="8">
+        <v>883</v>
+      </c>
       <c r="I53" s="2">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>795</v>
       </c>
       <c r="J53" s="2">
         <v>20210625</v>
@@ -9729,10 +9761,12 @@
       <c r="G54" s="8">
         <v>89</v>
       </c>
-      <c r="H54" s="8"/>
+      <c r="H54" s="8">
+        <v>899</v>
+      </c>
       <c r="I54" s="2">
         <f t="shared" si="0"/>
-        <v>-89</v>
+        <v>810</v>
       </c>
       <c r="J54" s="2">
         <v>20210625</v>
@@ -9767,10 +9801,12 @@
       <c r="G55" s="8">
         <v>88</v>
       </c>
-      <c r="H55" s="8"/>
+      <c r="H55" s="8">
+        <v>875</v>
+      </c>
       <c r="I55" s="2">
         <f t="shared" si="0"/>
-        <v>-88</v>
+        <v>787</v>
       </c>
       <c r="J55" s="2">
         <v>20210625</v>

</xml_diff>

<commit_message>
update and fix some things
</commit_message>
<xml_diff>
--- a/Data/LeachateData.xlsx
+++ b/Data/LeachateData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredflater/Desktop/Flater_soilColumnAnalysis/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredflater/Documents/2021_strips_soil_column/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE349893-0517-9648-817E-0A6E6082F87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EB9AF3-429F-3F4D-9349-C4ED08CCD803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16640" activeTab="4" xr2:uid="{BB50EEFD-D6E6-1446-BF52-B136C76F6CEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Rainfall 1" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="502">
   <si>
     <t>unique sample_id</t>
   </si>
@@ -1440,6 +1440,165 @@
   </si>
   <si>
     <t>SSCAMR00270</t>
+  </si>
+  <si>
+    <t>SSCAMR00271</t>
+  </si>
+  <si>
+    <t>SSCAMR00272</t>
+  </si>
+  <si>
+    <t>SSCAMR00273</t>
+  </si>
+  <si>
+    <t>SSCAMR00274</t>
+  </si>
+  <si>
+    <t>SSCAMR00275</t>
+  </si>
+  <si>
+    <t>SSCAMR00276</t>
+  </si>
+  <si>
+    <t>SSCAMR00277</t>
+  </si>
+  <si>
+    <t>SSCAMR00278</t>
+  </si>
+  <si>
+    <t>SSCAMR00279</t>
+  </si>
+  <si>
+    <t>SSCAMR00280</t>
+  </si>
+  <si>
+    <t>SSCAMR00281</t>
+  </si>
+  <si>
+    <t>SSCAMR00282</t>
+  </si>
+  <si>
+    <t>SSCAMR00283</t>
+  </si>
+  <si>
+    <t>SSCAMR00284</t>
+  </si>
+  <si>
+    <t>SSCAMR00285</t>
+  </si>
+  <si>
+    <t>SSCAMR00286</t>
+  </si>
+  <si>
+    <t>SSCAMR00287</t>
+  </si>
+  <si>
+    <t>SSCAMR00288</t>
+  </si>
+  <si>
+    <t>SSCAMR00289</t>
+  </si>
+  <si>
+    <t>SSCAMR00290</t>
+  </si>
+  <si>
+    <t>SSCAMR00291</t>
+  </si>
+  <si>
+    <t>SSCAMR00292</t>
+  </si>
+  <si>
+    <t>SSCAMR00293</t>
+  </si>
+  <si>
+    <t>SSCAMR00294</t>
+  </si>
+  <si>
+    <t>SSCAMR00295</t>
+  </si>
+  <si>
+    <t>SSCAMR00296</t>
+  </si>
+  <si>
+    <t>SSCAMR00297</t>
+  </si>
+  <si>
+    <t>SSCAMR00298</t>
+  </si>
+  <si>
+    <t>SSCAMR00299</t>
+  </si>
+  <si>
+    <t>SSCAMR00300</t>
+  </si>
+  <si>
+    <t>SSCAMR00301</t>
+  </si>
+  <si>
+    <t>SSCAMR00302</t>
+  </si>
+  <si>
+    <t>SSCAMR00303</t>
+  </si>
+  <si>
+    <t>SSCAMR00304</t>
+  </si>
+  <si>
+    <t>SSCAMR00305</t>
+  </si>
+  <si>
+    <t>SSCAMR00306</t>
+  </si>
+  <si>
+    <t>SSCAMR00307</t>
+  </si>
+  <si>
+    <t>SSCAMR00308</t>
+  </si>
+  <si>
+    <t>SSCAMR00309</t>
+  </si>
+  <si>
+    <t>SSCAMR00310</t>
+  </si>
+  <si>
+    <t>SSCAMR00311</t>
+  </si>
+  <si>
+    <t>SSCAMR00312</t>
+  </si>
+  <si>
+    <t>SSCAMR00313</t>
+  </si>
+  <si>
+    <t>SSCAMR00314</t>
+  </si>
+  <si>
+    <t>SSCAMR00315</t>
+  </si>
+  <si>
+    <t>SSCAMR00316</t>
+  </si>
+  <si>
+    <t>SSCAMR00317</t>
+  </si>
+  <si>
+    <t>SSCAMR00318</t>
+  </si>
+  <si>
+    <t>SSCAMR00319</t>
+  </si>
+  <si>
+    <t>SSCAMR00320</t>
+  </si>
+  <si>
+    <t>SSCAMR00321</t>
+  </si>
+  <si>
+    <t>SSCAMR00322</t>
+  </si>
+  <si>
+    <t>SSCAMR00323</t>
   </si>
 </sst>
 </file>
@@ -1468,7 +1627,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1485,12 +1644,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1545,7 +1698,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5719,7 +5872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7CF24D-EF41-5241-906E-DAD6D3AC4CE4}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C19" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -7744,8 +7897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556C630F-CED0-3C49-9F7A-3D77E458B865}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9251,7 +9404,7 @@
         <v>322</v>
       </c>
       <c r="D38" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E38" s="2">
         <v>4</v>
@@ -9260,17 +9413,17 @@
         <v>1000</v>
       </c>
       <c r="G38" s="8">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H38" s="8">
-        <v>1000</v>
+        <v>827</v>
       </c>
       <c r="I38" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>723</v>
       </c>
       <c r="J38" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>230</v>
@@ -9291,7 +9444,7 @@
         <v>323</v>
       </c>
       <c r="D39" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E39" s="2">
         <v>4</v>
@@ -9300,17 +9453,17 @@
         <v>1000</v>
       </c>
       <c r="G39" s="8">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="H39" s="8">
-        <v>1000</v>
+        <v>827</v>
       </c>
       <c r="I39" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>738</v>
       </c>
       <c r="J39" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>230</v>
@@ -9331,7 +9484,7 @@
         <v>324</v>
       </c>
       <c r="D40" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E40" s="2">
         <v>4</v>
@@ -9340,17 +9493,17 @@
         <v>1000</v>
       </c>
       <c r="G40" s="8">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H40" s="8">
-        <v>1000</v>
+        <v>893</v>
       </c>
       <c r="I40" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>805</v>
       </c>
       <c r="J40" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>230</v>
@@ -9371,7 +9524,7 @@
         <v>325</v>
       </c>
       <c r="D41" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E41" s="2">
         <v>4</v>
@@ -9380,17 +9533,17 @@
         <v>1000</v>
       </c>
       <c r="G41" s="8">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H41" s="8">
-        <v>1000</v>
+        <v>856</v>
       </c>
       <c r="I41" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>768</v>
       </c>
       <c r="J41" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>230</v>
@@ -9411,7 +9564,7 @@
         <v>326</v>
       </c>
       <c r="D42" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E42" s="2">
         <v>4</v>
@@ -9420,17 +9573,17 @@
         <v>1000</v>
       </c>
       <c r="G42" s="8">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H42" s="8">
-        <v>1000</v>
+        <v>817</v>
       </c>
       <c r="I42" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>729</v>
       </c>
       <c r="J42" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>230</v>
@@ -9451,7 +9604,7 @@
         <v>327</v>
       </c>
       <c r="D43" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E43" s="2">
         <v>4</v>
@@ -9460,17 +9613,17 @@
         <v>1000</v>
       </c>
       <c r="G43" s="8">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="H43" s="8">
-        <v>1000</v>
+        <v>817</v>
       </c>
       <c r="I43" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>728</v>
       </c>
       <c r="J43" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>230</v>
@@ -9491,7 +9644,7 @@
         <v>328</v>
       </c>
       <c r="D44" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E44" s="2">
         <v>4</v>
@@ -9500,17 +9653,17 @@
         <v>1000</v>
       </c>
       <c r="G44" s="8">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H44" s="8">
-        <v>1000</v>
+        <v>896</v>
       </c>
       <c r="I44" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>808</v>
       </c>
       <c r="J44" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>230</v>
@@ -9531,7 +9684,7 @@
         <v>329</v>
       </c>
       <c r="D45" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E45" s="2">
         <v>4</v>
@@ -9540,17 +9693,17 @@
         <v>1000</v>
       </c>
       <c r="G45" s="8">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H45" s="8">
-        <v>1000</v>
+        <v>808</v>
       </c>
       <c r="I45" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>720</v>
       </c>
       <c r="J45" s="2">
-        <v>20210626</v>
+        <v>20210628</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>230</v>
@@ -9571,7 +9724,7 @@
         <v>330</v>
       </c>
       <c r="D46" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E46" s="2">
         <v>4</v>
@@ -9580,17 +9733,17 @@
         <v>1000</v>
       </c>
       <c r="G46" s="8">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H46" s="8">
-        <v>1000</v>
+        <v>808</v>
       </c>
       <c r="I46" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>720</v>
       </c>
       <c r="J46" s="2">
-        <v>20210626</v>
+        <v>20210628</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>230</v>
@@ -9611,7 +9764,7 @@
         <v>331</v>
       </c>
       <c r="D47" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E47" s="2">
         <v>4</v>
@@ -9620,17 +9773,17 @@
         <v>1000</v>
       </c>
       <c r="G47" s="8">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H47" s="8">
-        <v>1000</v>
+        <v>846</v>
       </c>
       <c r="I47" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>758</v>
       </c>
       <c r="J47" s="2">
-        <v>20210626</v>
+        <v>20210628</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>230</v>
@@ -9651,7 +9804,7 @@
         <v>332</v>
       </c>
       <c r="D48" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E48" s="2">
         <v>4</v>
@@ -9660,17 +9813,17 @@
         <v>1000</v>
       </c>
       <c r="G48" s="8">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="H48" s="8">
-        <v>1000</v>
+        <v>903</v>
       </c>
       <c r="I48" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>814</v>
       </c>
       <c r="J48" s="2">
-        <v>20210626</v>
+        <v>20210628</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>230</v>
@@ -9691,7 +9844,7 @@
         <v>333</v>
       </c>
       <c r="D49" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E49" s="2">
         <v>4</v>
@@ -9700,17 +9853,17 @@
         <v>1000</v>
       </c>
       <c r="G49" s="8">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H49" s="8">
-        <v>1000</v>
+        <v>868</v>
       </c>
       <c r="I49" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>765</v>
       </c>
       <c r="J49" s="2">
-        <v>20210626</v>
+        <v>20210628</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>230</v>
@@ -9731,7 +9884,7 @@
         <v>334</v>
       </c>
       <c r="D50" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E50" s="2">
         <v>4</v>
@@ -9740,17 +9893,17 @@
         <v>1000</v>
       </c>
       <c r="G50" s="8">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="H50" s="8">
-        <v>1000</v>
+        <v>915</v>
       </c>
       <c r="I50" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>826</v>
       </c>
       <c r="J50" s="2">
-        <v>20210626</v>
+        <v>20210628</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>230</v>
@@ -9771,7 +9924,7 @@
         <v>335</v>
       </c>
       <c r="D51" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E51" s="2">
         <v>4</v>
@@ -9780,17 +9933,17 @@
         <v>1000</v>
       </c>
       <c r="G51" s="8">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="H51" s="8">
-        <v>1000</v>
+        <v>863</v>
       </c>
       <c r="I51" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>774</v>
       </c>
       <c r="J51" s="2">
-        <v>20210626</v>
+        <v>20210628</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>230</v>
@@ -9811,7 +9964,7 @@
         <v>336</v>
       </c>
       <c r="D52" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E52" s="2">
         <v>4</v>
@@ -9820,17 +9973,17 @@
         <v>1000</v>
       </c>
       <c r="G52" s="8">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H52" s="8">
-        <v>1000</v>
+        <v>878</v>
       </c>
       <c r="I52" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>790</v>
       </c>
       <c r="J52" s="2">
-        <v>20210626</v>
+        <v>20210628</v>
       </c>
       <c r="K52" s="2" t="s">
         <v>230</v>
@@ -9851,7 +10004,7 @@
         <v>337</v>
       </c>
       <c r="D53" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E53" s="2">
         <v>4</v>
@@ -9860,17 +10013,17 @@
         <v>1000</v>
       </c>
       <c r="G53" s="8">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H53" s="8">
-        <v>1000</v>
+        <v>883</v>
       </c>
       <c r="I53" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>795</v>
       </c>
       <c r="J53" s="2">
-        <v>20210626</v>
+        <v>20210628</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>230</v>
@@ -9891,7 +10044,7 @@
         <v>338</v>
       </c>
       <c r="D54" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E54" s="2">
         <v>4</v>
@@ -9900,17 +10053,17 @@
         <v>1000</v>
       </c>
       <c r="G54" s="8">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="H54" s="8">
-        <v>1000</v>
+        <v>899</v>
       </c>
       <c r="I54" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>810</v>
       </c>
       <c r="J54" s="2">
-        <v>20210626</v>
+        <v>20210628</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>230</v>
@@ -9931,7 +10084,7 @@
         <v>339</v>
       </c>
       <c r="D55" s="2">
-        <v>20210626</v>
+        <v>20210625</v>
       </c>
       <c r="E55" s="2">
         <v>4</v>
@@ -9940,17 +10093,17 @@
         <v>1000</v>
       </c>
       <c r="G55" s="8">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H55" s="8">
-        <v>1000</v>
+        <v>875</v>
       </c>
       <c r="I55" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>787</v>
       </c>
       <c r="J55" s="2">
-        <v>20210626</v>
+        <v>20210628</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>230</v>
@@ -9968,12 +10121,1938 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C5F78B-ED0A-A94A-92EC-0E12CA5D830D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="2">
+        <v>88</v>
+      </c>
+      <c r="H2" s="2">
+        <v>889</v>
+      </c>
+      <c r="I2" s="2">
+        <f>H2-G2</f>
+        <v>801</v>
+      </c>
+      <c r="J2" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="2">
+        <v>101</v>
+      </c>
+      <c r="H3" s="2">
+        <v>860</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I55" si="0">H3-G3</f>
+        <v>759</v>
+      </c>
+      <c r="J3" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="2">
+        <v>88</v>
+      </c>
+      <c r="H4" s="2">
+        <v>899</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="0"/>
+        <v>811</v>
+      </c>
+      <c r="J4" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D5" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G5" s="2">
+        <v>101</v>
+      </c>
+      <c r="H5" s="2">
+        <v>864</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="0"/>
+        <v>763</v>
+      </c>
+      <c r="J5" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D6" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G6" s="2">
+        <v>90</v>
+      </c>
+      <c r="H6" s="2">
+        <v>875</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="0"/>
+        <v>785</v>
+      </c>
+      <c r="J6" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D7" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="2">
+        <v>91</v>
+      </c>
+      <c r="H7" s="2">
+        <v>813</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="0"/>
+        <v>722</v>
+      </c>
+      <c r="J7" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D8" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="2">
+        <v>91</v>
+      </c>
+      <c r="H8" s="2">
+        <v>889</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>798</v>
+      </c>
+      <c r="J8" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D9" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G9" s="2">
+        <v>89</v>
+      </c>
+      <c r="H9" s="2">
+        <v>848</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="0"/>
+        <v>759</v>
+      </c>
+      <c r="J9" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D10" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G10" s="2">
+        <v>90</v>
+      </c>
+      <c r="H10" s="2">
+        <v>912</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="0"/>
+        <v>822</v>
+      </c>
+      <c r="J10" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D11" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G11" s="2">
+        <v>89</v>
+      </c>
+      <c r="H11" s="2">
+        <v>816</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="0"/>
+        <v>727</v>
+      </c>
+      <c r="J11" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D12" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G12" s="2">
+        <v>90</v>
+      </c>
+      <c r="H12" s="2">
+        <v>940</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
+        <v>850</v>
+      </c>
+      <c r="J12" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G13" s="2">
+        <v>89</v>
+      </c>
+      <c r="H13" s="2">
+        <v>851</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="0"/>
+        <v>762</v>
+      </c>
+      <c r="J13" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D14" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G14" s="2">
+        <v>91</v>
+      </c>
+      <c r="H14" s="2">
+        <v>925</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="0"/>
+        <v>834</v>
+      </c>
+      <c r="J14" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D15" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G15" s="2">
+        <v>89</v>
+      </c>
+      <c r="H15" s="2">
+        <v>877</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="0"/>
+        <v>788</v>
+      </c>
+      <c r="J15" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D16" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
+      <c r="F16" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G16" s="2">
+        <v>90</v>
+      </c>
+      <c r="H16" s="2">
+        <v>912</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="0"/>
+        <v>822</v>
+      </c>
+      <c r="J16" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D17" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G17" s="2">
+        <v>89</v>
+      </c>
+      <c r="H17" s="2">
+        <v>865</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="0"/>
+        <v>776</v>
+      </c>
+      <c r="J17" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D18" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G18" s="2">
+        <v>88</v>
+      </c>
+      <c r="H18" s="2">
+        <v>899</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="0"/>
+        <v>811</v>
+      </c>
+      <c r="J18" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G19" s="2">
+        <v>105</v>
+      </c>
+      <c r="H19" s="2">
+        <v>846</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="0"/>
+        <v>741</v>
+      </c>
+      <c r="J19" s="2">
+        <v>20210628</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="F20" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2">
+        <v>5</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2">
+        <v>5</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
+      <c r="F25" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2">
+        <v>5</v>
+      </c>
+      <c r="F26" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2">
+        <v>5</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2">
+        <v>5</v>
+      </c>
+      <c r="F28" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
+        <v>5</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2">
+        <v>5</v>
+      </c>
+      <c r="F31" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2">
+        <v>5</v>
+      </c>
+      <c r="F32" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2">
+        <v>5</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2">
+        <v>5</v>
+      </c>
+      <c r="F34" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2">
+        <v>5</v>
+      </c>
+      <c r="F35" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2">
+        <v>5</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2">
+        <v>5</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2">
+        <v>5</v>
+      </c>
+      <c r="F38" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2">
+        <v>5</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2">
+        <v>5</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2">
+        <v>5</v>
+      </c>
+      <c r="F41" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2">
+        <v>5</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2">
+        <v>5</v>
+      </c>
+      <c r="F43" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2">
+        <v>5</v>
+      </c>
+      <c r="F44" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2">
+        <v>5</v>
+      </c>
+      <c r="F45" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2">
+        <v>5</v>
+      </c>
+      <c r="F46" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2">
+        <v>5</v>
+      </c>
+      <c r="F47" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2">
+        <v>5</v>
+      </c>
+      <c r="F48" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2">
+        <v>5</v>
+      </c>
+      <c r="F49" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2">
+        <v>5</v>
+      </c>
+      <c r="F50" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2">
+        <v>5</v>
+      </c>
+      <c r="F51" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2">
+        <v>5</v>
+      </c>
+      <c r="F52" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2">
+        <v>5</v>
+      </c>
+      <c r="F53" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2">
+        <v>5</v>
+      </c>
+      <c r="F54" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2">
+        <v>5</v>
+      </c>
+      <c r="F55" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>